<commit_message>
Changed the header in the Main Dashboard file
</commit_message>
<xml_diff>
--- a/actual_energy.xlsx
+++ b/actual_energy.xlsx
@@ -448,13 +448,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>66219</v>
+        <v>68377</v>
       </c>
       <c r="C2" t="n">
-        <v>4978.75</v>
+        <v>5373.441499999999</v>
       </c>
       <c r="D2" t="n">
-        <v>61240.25</v>
+        <v>63003.5585</v>
       </c>
     </row>
     <row r="3">
@@ -462,13 +462,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>64309</v>
+        <v>65754</v>
       </c>
       <c r="C3" t="n">
-        <v>4881.803465346536</v>
+        <v>5250.357</v>
       </c>
       <c r="D3" t="n">
-        <v>59427.19653465346</v>
+        <v>60503.643</v>
       </c>
     </row>
     <row r="4">
@@ -476,13 +476,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>62149</v>
+        <v>63452</v>
       </c>
       <c r="C4" t="n">
-        <v>4806.189603960396</v>
+        <v>5171.886999999999</v>
       </c>
       <c r="D4" t="n">
-        <v>57342.8103960396</v>
+        <v>58280.113</v>
       </c>
     </row>
     <row r="5">
@@ -490,13 +490,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>60657</v>
+        <v>61778</v>
       </c>
       <c r="C5" t="n">
-        <v>4777.004455445544</v>
+        <v>5107.980499999999</v>
       </c>
       <c r="D5" t="n">
-        <v>55879.99554455445</v>
+        <v>56670.0195</v>
       </c>
     </row>
     <row r="6">
@@ -504,13 +504,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>62958</v>
+        <v>63701</v>
       </c>
       <c r="C6" t="n">
-        <v>4817.022277227723</v>
+        <v>5104.393</v>
       </c>
       <c r="D6" t="n">
-        <v>58140.97772277228</v>
+        <v>58596.607</v>
       </c>
     </row>
     <row r="7">
@@ -518,13 +518,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>65273</v>
+        <v>66921</v>
       </c>
       <c r="C7" t="n">
-        <v>4993.585148514851</v>
+        <v>5230.476999999999</v>
       </c>
       <c r="D7" t="n">
-        <v>60279.41485148515</v>
+        <v>61690.523</v>
       </c>
     </row>
     <row r="8">
@@ -532,13 +532,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>64219</v>
+        <v>65559</v>
       </c>
       <c r="C8" t="n">
-        <v>5791.976732673267</v>
+        <v>5902.879499999999</v>
       </c>
       <c r="D8" t="n">
-        <v>58427.02326732673</v>
+        <v>59656.1205</v>
       </c>
     </row>
     <row r="9">
@@ -546,13 +546,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>62558</v>
+        <v>77302</v>
       </c>
       <c r="C9" t="n">
-        <v>6508.679702970297</v>
+        <v>7037.001999999999</v>
       </c>
       <c r="D9" t="n">
-        <v>56049.32029702971</v>
+        <v>70264.99800000001</v>
       </c>
     </row>
     <row r="10">
@@ -560,13 +560,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>92325</v>
+        <v>94353</v>
       </c>
       <c r="C10" t="n">
-        <v>8013.319306930694</v>
+        <v>8592.440500000001</v>
       </c>
       <c r="D10" t="n">
-        <v>84311.6806930693</v>
+        <v>85760.5595</v>
       </c>
     </row>
     <row r="11">
@@ -574,13 +574,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>104189</v>
+        <v>84696</v>
       </c>
       <c r="C11" t="n">
-        <v>13327.75396039604</v>
+        <v>14095.0215</v>
       </c>
       <c r="D11" t="n">
-        <v>90861.24603960395</v>
+        <v>70600.9785</v>
       </c>
     </row>
     <row r="12">
@@ -588,13 +588,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>87429</v>
+        <v>105351</v>
       </c>
       <c r="C12" t="n">
-        <v>14912.39801980198</v>
+        <v>15828.8445</v>
       </c>
       <c r="D12" t="n">
-        <v>72516.60198019801</v>
+        <v>89522.15549999999</v>
       </c>
     </row>
     <row r="13">
@@ -602,13 +602,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>88764</v>
+        <v>106616</v>
       </c>
       <c r="C13" t="n">
-        <v>14866.84603960396</v>
+        <v>15449.287</v>
       </c>
       <c r="D13" t="n">
-        <v>73897.15396039604</v>
+        <v>91166.713</v>
       </c>
     </row>
     <row r="14">
@@ -616,27 +616,24 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>69428</v>
+        <v>105965</v>
       </c>
       <c r="C14" t="n">
-        <v>15166.13415841584</v>
+        <v>15803.2595</v>
       </c>
       <c r="D14" t="n">
-        <v>54261.86584158416</v>
+        <v>90161.7405</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
         <v>14</v>
       </c>
-      <c r="B15" t="n">
-        <v>56205</v>
-      </c>
       <c r="C15" t="n">
-        <v>15342.26732673267</v>
+        <v>15862.028</v>
       </c>
       <c r="D15" t="n">
-        <v>40862.73267326733</v>
+        <v>74053.73267326732</v>
       </c>
     </row>
     <row r="16">
@@ -644,10 +641,10 @@
         <v>15</v>
       </c>
       <c r="C16" t="n">
-        <v>15647.49851485148</v>
+        <v>16032.3205</v>
       </c>
       <c r="D16" t="n">
-        <v>58895.0615</v>
+        <v>95771.50148514852</v>
       </c>
     </row>
     <row r="17">
@@ -655,10 +652,10 @@
         <v>16</v>
       </c>
       <c r="C17" t="n">
-        <v>15775.31782178218</v>
+        <v>16559.4275</v>
       </c>
       <c r="D17" t="n">
-        <v>56450.1975</v>
+        <v>84547.68217821782</v>
       </c>
     </row>
     <row r="18">
@@ -666,10 +663,10 @@
         <v>17</v>
       </c>
       <c r="C18" t="n">
-        <v>16246.4004950495</v>
+        <v>16683.57249999999</v>
       </c>
       <c r="D18" t="n">
-        <v>67467.57000000001</v>
+        <v>59953.5995049505</v>
       </c>
     </row>
     <row r="19">
@@ -677,7 +674,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="n">
-        <v>15938.57376237624</v>
+        <v>16252.82049999999</v>
       </c>
       <c r="D19" t="n">
         <v>72066.9185</v>
@@ -688,7 +685,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>15549.6094059406</v>
+        <v>15546.958</v>
       </c>
       <c r="D20" t="n">
         <v>74173.3315</v>
@@ -699,7 +696,7 @@
         <v>20</v>
       </c>
       <c r="C21" t="n">
-        <v>13984.29504950495</v>
+        <v>13748.4165</v>
       </c>
       <c r="D21" t="n">
         <v>72400.7075</v>
@@ -710,7 +707,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="n">
-        <v>12412.51089108911</v>
+        <v>12030.7215</v>
       </c>
       <c r="D22" t="n">
         <v>70217.473</v>
@@ -721,7 +718,7 @@
         <v>22</v>
       </c>
       <c r="C23" t="n">
-        <v>9434.527227722774</v>
+        <v>9319.645999999999</v>
       </c>
       <c r="D23" t="n">
         <v>21309.33</v>
@@ -732,7 +729,7 @@
         <v>23</v>
       </c>
       <c r="C24" t="n">
-        <v>6390.105940594059</v>
+        <v>6308.333499999995</v>
       </c>
       <c r="D24" t="n">
         <v>69506.016</v>
@@ -743,7 +740,7 @@
         <v>24</v>
       </c>
       <c r="C25" t="n">
-        <v>5462.339108910891</v>
+        <v>5687.261999999999</v>
       </c>
       <c r="D25" t="n">
         <v>44605.08100000001</v>

</xml_diff>

<commit_message>
Changed the page icon
</commit_message>
<xml_diff>
--- a/actual_energy.xlsx
+++ b/actual_energy.xlsx
@@ -574,13 +574,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>84696</v>
+        <v>103695</v>
       </c>
       <c r="C11" t="n">
         <v>14095.0215</v>
       </c>
       <c r="D11" t="n">
-        <v>70600.9785</v>
+        <v>89599.9785</v>
       </c>
     </row>
     <row r="12">
@@ -588,13 +588,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>105351</v>
+        <v>107380</v>
       </c>
       <c r="C12" t="n">
         <v>15828.8445</v>
       </c>
       <c r="D12" t="n">
-        <v>89522.15549999999</v>
+        <v>91551.15549999999</v>
       </c>
     </row>
     <row r="13">

</xml_diff>

<commit_message>
Modified Main Dashboard file
</commit_message>
<xml_diff>
--- a/actual_energy.xlsx
+++ b/actual_energy.xlsx
@@ -602,13 +602,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>106616</v>
+        <v>108706</v>
       </c>
       <c r="C13" t="n">
         <v>15449.287</v>
       </c>
       <c r="D13" t="n">
-        <v>91166.713</v>
+        <v>93256.713</v>
       </c>
     </row>
     <row r="14">
@@ -616,46 +616,55 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>105965</v>
+        <v>108006</v>
       </c>
       <c r="C14" t="n">
         <v>15803.2595</v>
       </c>
       <c r="D14" t="n">
-        <v>90161.7405</v>
+        <v>92202.7405</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
         <v>14</v>
       </c>
+      <c r="B15" t="n">
+        <v>83578</v>
+      </c>
       <c r="C15" t="n">
         <v>15862.028</v>
       </c>
       <c r="D15" t="n">
-        <v>74053.73267326732</v>
+        <v>67715.97199999999</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
         <v>15</v>
       </c>
+      <c r="B16" t="n">
+        <v>83212</v>
+      </c>
       <c r="C16" t="n">
         <v>16032.3205</v>
       </c>
       <c r="D16" t="n">
-        <v>95771.50148514852</v>
+        <v>67179.6795</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
         <v>16</v>
       </c>
+      <c r="B17" t="n">
+        <v>79873</v>
+      </c>
       <c r="C17" t="n">
         <v>16559.4275</v>
       </c>
       <c r="D17" t="n">
-        <v>84547.68217821782</v>
+        <v>63313.57249999999</v>
       </c>
     </row>
     <row r="18">

</xml_diff>

<commit_message>
Modified the Main Dashboard file
</commit_message>
<xml_diff>
--- a/actual_energy.xlsx
+++ b/actual_energy.xlsx
@@ -448,13 +448,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>78805</v>
+        <v>78622</v>
       </c>
       <c r="C2" t="n">
-        <v>5569.423999999999</v>
+        <v>5444.512500000001</v>
       </c>
       <c r="D2" t="n">
-        <v>73235.576</v>
+        <v>73177.4875</v>
       </c>
     </row>
     <row r="3">
@@ -462,13 +462,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>74694</v>
+        <v>75199</v>
       </c>
       <c r="C3" t="n">
-        <v>5443.025</v>
+        <v>5387.3435</v>
       </c>
       <c r="D3" t="n">
-        <v>69250.97500000001</v>
+        <v>69811.6565</v>
       </c>
     </row>
     <row r="4">
@@ -476,13 +476,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>71872</v>
+        <v>69820</v>
       </c>
       <c r="C4" t="n">
-        <v>5335.7675</v>
+        <v>5357.2225</v>
       </c>
       <c r="D4" t="n">
-        <v>66536.2325</v>
+        <v>64462.7775</v>
       </c>
     </row>
     <row r="5">
@@ -490,13 +490,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>68930</v>
+        <v>69709</v>
       </c>
       <c r="C5" t="n">
-        <v>5326.111</v>
+        <v>5289.154500000001</v>
       </c>
       <c r="D5" t="n">
-        <v>63603.889</v>
+        <v>64419.8455</v>
       </c>
     </row>
     <row r="6">
@@ -504,13 +504,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>68060</v>
+        <v>69148</v>
       </c>
       <c r="C6" t="n">
-        <v>5353.5615</v>
+        <v>5361.8285</v>
       </c>
       <c r="D6" t="n">
-        <v>62706.4385</v>
+        <v>63786.1715</v>
       </c>
     </row>
     <row r="7">
@@ -518,13 +518,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>68909</v>
+        <v>71026</v>
       </c>
       <c r="C7" t="n">
-        <v>5400.717</v>
+        <v>5442.6015</v>
       </c>
       <c r="D7" t="n">
-        <v>63508.283</v>
+        <v>65583.3985</v>
       </c>
     </row>
     <row r="8">
@@ -532,13 +532,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>68628</v>
+        <v>69369</v>
       </c>
       <c r="C8" t="n">
-        <v>5986.228500000001</v>
+        <v>5816.530999999999</v>
       </c>
       <c r="D8" t="n">
-        <v>62641.7715</v>
+        <v>63552.469</v>
       </c>
     </row>
     <row r="9">
@@ -546,13 +546,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>77034</v>
+        <v>83438</v>
       </c>
       <c r="C9" t="n">
-        <v>6774.907999999999</v>
+        <v>7034.6115</v>
       </c>
       <c r="D9" t="n">
-        <v>70259.092</v>
+        <v>76403.3885</v>
       </c>
     </row>
     <row r="10">
@@ -560,41 +560,35 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>72266</v>
+        <v>67948</v>
       </c>
       <c r="C10" t="n">
-        <v>8159.217500000001</v>
+        <v>8596.6895</v>
       </c>
       <c r="D10" t="n">
-        <v>64106.7825</v>
+        <v>59351.3105</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
         <v>10</v>
       </c>
-      <c r="B11" t="n">
-        <v>80854</v>
-      </c>
       <c r="C11" t="n">
-        <v>13111.5495</v>
+        <v>13942.873</v>
       </c>
       <c r="D11" t="n">
-        <v>67742.45050000001</v>
+        <v>99192.12700000001</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
         <v>11</v>
       </c>
-      <c r="B12" t="n">
-        <v>67889</v>
-      </c>
       <c r="C12" t="n">
-        <v>15041.6385</v>
+        <v>15769.3095</v>
       </c>
       <c r="D12" t="n">
-        <v>52847.3615</v>
+        <v>99767.6905</v>
       </c>
     </row>
     <row r="13">
@@ -602,10 +596,10 @@
         <v>12</v>
       </c>
       <c r="C13" t="n">
-        <v>15360.8175</v>
+        <v>15209.229</v>
       </c>
       <c r="D13" t="n">
-        <v>96998.807575</v>
+        <v>100144.771</v>
       </c>
     </row>
     <row r="14">
@@ -613,10 +607,10 @@
         <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>15438.7275</v>
+        <v>15159.795</v>
       </c>
       <c r="D14" t="n">
-        <v>96596.9025425</v>
+        <v>101117.205</v>
       </c>
     </row>
     <row r="15">
@@ -624,10 +618,10 @@
         <v>14</v>
       </c>
       <c r="C15" t="n">
-        <v>15496.474</v>
+        <v>15449.4445</v>
       </c>
       <c r="D15" t="n">
-        <v>100447.1062675</v>
+        <v>108724.5555</v>
       </c>
     </row>
     <row r="16">
@@ -635,10 +629,10 @@
         <v>15</v>
       </c>
       <c r="C16" t="n">
-        <v>15736.574</v>
+        <v>15588.433</v>
       </c>
       <c r="D16" t="n">
-        <v>101020.1465775</v>
+        <v>103763.567</v>
       </c>
     </row>
     <row r="17">
@@ -646,10 +640,10 @@
         <v>16</v>
       </c>
       <c r="C17" t="n">
-        <v>16203.3305</v>
+        <v>16020.6585</v>
       </c>
       <c r="D17" t="n">
-        <v>97530.9176425</v>
+        <v>101211.3415</v>
       </c>
     </row>
     <row r="18">
@@ -657,10 +651,10 @@
         <v>17</v>
       </c>
       <c r="C18" t="n">
-        <v>16035.0225</v>
+        <v>16262.3825</v>
       </c>
       <c r="D18" t="n">
-        <v>89225.8361625</v>
+        <v>93839.61749999999</v>
       </c>
     </row>
     <row r="19">
@@ -668,10 +662,10 @@
         <v>18</v>
       </c>
       <c r="C19" t="n">
-        <v>15489.1135</v>
+        <v>15862.609</v>
       </c>
       <c r="D19" t="n">
-        <v>72066.9185</v>
+        <v>88583.391</v>
       </c>
     </row>
     <row r="20">
@@ -679,10 +673,10 @@
         <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>15075.4555</v>
+        <v>14887.418</v>
       </c>
       <c r="D20" t="n">
-        <v>74173.3315</v>
+        <v>89024.58199999999</v>
       </c>
     </row>
     <row r="21">
@@ -690,10 +684,10 @@
         <v>20</v>
       </c>
       <c r="C21" t="n">
-        <v>13277.7365</v>
+        <v>13341.0375</v>
       </c>
       <c r="D21" t="n">
-        <v>72400.7075</v>
+        <v>87063.96249999999</v>
       </c>
     </row>
     <row r="22">
@@ -701,10 +695,10 @@
         <v>21</v>
       </c>
       <c r="C22" t="n">
-        <v>11738.566</v>
+        <v>11837.672</v>
       </c>
       <c r="D22" t="n">
-        <v>70217.473</v>
+        <v>85910.32799999999</v>
       </c>
     </row>
     <row r="23">
@@ -712,10 +706,10 @@
         <v>22</v>
       </c>
       <c r="C23" t="n">
-        <v>8937.529999999999</v>
+        <v>9490.991999999998</v>
       </c>
       <c r="D23" t="n">
-        <v>21309.33</v>
+        <v>84684.008</v>
       </c>
     </row>
     <row r="24">
@@ -723,10 +717,10 @@
         <v>23</v>
       </c>
       <c r="C24" t="n">
-        <v>5960.1675</v>
+        <v>6891.794</v>
       </c>
       <c r="D24" t="n">
-        <v>69506.016</v>
+        <v>81619.20600000001</v>
       </c>
     </row>
     <row r="25">
@@ -734,10 +728,10 @@
         <v>24</v>
       </c>
       <c r="C25" t="n">
-        <v>5052.110000000001</v>
+        <v>5770.9715</v>
       </c>
       <c r="D25" t="n">
-        <v>44605.08100000001</v>
+        <v>52348.0285</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified and deleted some files
</commit_message>
<xml_diff>
--- a/actual_energy.xlsx
+++ b/actual_energy.xlsx
@@ -448,13 +448,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>67078</v>
+        <v>72056</v>
       </c>
       <c r="C2" t="n">
-        <v>5554.7135</v>
+        <v>5516.6335</v>
       </c>
       <c r="D2" t="n">
-        <v>61523.2865</v>
+        <v>66539.3665</v>
       </c>
     </row>
     <row r="3">
@@ -462,13 +462,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>64200</v>
+        <v>69308</v>
       </c>
       <c r="C3" t="n">
-        <v>5359.343500000001</v>
+        <v>5387.312</v>
       </c>
       <c r="D3" t="n">
-        <v>58840.6565</v>
+        <v>63920.688</v>
       </c>
     </row>
     <row r="4">
@@ -476,13 +476,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>62248</v>
+        <v>65612</v>
       </c>
       <c r="C4" t="n">
-        <v>5311.7505</v>
+        <v>5339.824000000001</v>
       </c>
       <c r="D4" t="n">
-        <v>56936.2495</v>
+        <v>60272.176</v>
       </c>
     </row>
     <row r="5">
@@ -490,13 +490,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>60861</v>
+        <v>64269</v>
       </c>
       <c r="C5" t="n">
-        <v>5299.952</v>
+        <v>5306.819000000001</v>
       </c>
       <c r="D5" t="n">
-        <v>55561.048</v>
+        <v>58962.181</v>
       </c>
     </row>
     <row r="6">
@@ -504,13 +504,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>55982</v>
+        <v>65136</v>
       </c>
       <c r="C6" t="n">
-        <v>5293.1515</v>
+        <v>5338.83</v>
       </c>
       <c r="D6" t="n">
-        <v>50688.8485</v>
+        <v>59797.17</v>
       </c>
     </row>
     <row r="7">
@@ -518,13 +518,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>61100</v>
+        <v>71065</v>
       </c>
       <c r="C7" t="n">
-        <v>5324.76</v>
+        <v>5422.714499999999</v>
       </c>
       <c r="D7" t="n">
-        <v>55775.24</v>
+        <v>65642.2855</v>
       </c>
     </row>
     <row r="8">
@@ -532,13 +532,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>61451</v>
+        <v>70049</v>
       </c>
       <c r="C8" t="n">
-        <v>6198.4755</v>
+        <v>5875.107</v>
       </c>
       <c r="D8" t="n">
-        <v>55252.5245</v>
+        <v>64173.893</v>
       </c>
     </row>
     <row r="9">
@@ -546,13 +546,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>65951</v>
+        <v>80484</v>
       </c>
       <c r="C9" t="n">
-        <v>6632.370499999999</v>
+        <v>7214.4275</v>
       </c>
       <c r="D9" t="n">
-        <v>59318.6295</v>
+        <v>73269.57249999999</v>
       </c>
     </row>
     <row r="10">
@@ -560,13 +560,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>75046</v>
+        <v>94725</v>
       </c>
       <c r="C10" t="n">
-        <v>7985.929</v>
+        <v>8467.018</v>
       </c>
       <c r="D10" t="n">
-        <v>67060.071</v>
+        <v>86257.982</v>
       </c>
     </row>
     <row r="11">
@@ -574,13 +574,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>84778</v>
+        <v>104123</v>
       </c>
       <c r="C11" t="n">
-        <v>13162.0615</v>
+        <v>13640.6165</v>
       </c>
       <c r="D11" t="n">
-        <v>71615.9385</v>
+        <v>90482.3835</v>
       </c>
     </row>
     <row r="12">
@@ -588,13 +588,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>87637</v>
+        <v>110312</v>
       </c>
       <c r="C12" t="n">
-        <v>15499.911</v>
+        <v>15763.02</v>
       </c>
       <c r="D12" t="n">
-        <v>72137.08900000001</v>
+        <v>94548.98</v>
       </c>
     </row>
     <row r="13">
@@ -602,13 +602,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>88210</v>
+        <v>111321</v>
       </c>
       <c r="C13" t="n">
-        <v>15978.718</v>
+        <v>15072.0395</v>
       </c>
       <c r="D13" t="n">
-        <v>72231.28200000001</v>
+        <v>96248.9605</v>
       </c>
     </row>
     <row r="14">
@@ -616,13 +616,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>90838</v>
+        <v>109259</v>
       </c>
       <c r="C14" t="n">
-        <v>15949.85</v>
+        <v>15259.6675</v>
       </c>
       <c r="D14" t="n">
-        <v>74888.14999999999</v>
+        <v>93999.3325</v>
       </c>
     </row>
     <row r="15">
@@ -630,13 +630,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>94152</v>
+        <v>113429</v>
       </c>
       <c r="C15" t="n">
-        <v>16112.4845</v>
+        <v>15815.744</v>
       </c>
       <c r="D15" t="n">
-        <v>78039.51549999999</v>
+        <v>97613.25599999999</v>
       </c>
     </row>
     <row r="16">
@@ -644,13 +644,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>96251</v>
+        <v>114542</v>
       </c>
       <c r="C16" t="n">
-        <v>16701.4645</v>
+        <v>15955.3275</v>
       </c>
       <c r="D16" t="n">
-        <v>79549.5355</v>
+        <v>98586.6725</v>
       </c>
     </row>
     <row r="17">
@@ -658,13 +658,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>96983</v>
+        <v>99426</v>
       </c>
       <c r="C17" t="n">
-        <v>16519.7305</v>
+        <v>16114.0735</v>
       </c>
       <c r="D17" t="n">
-        <v>80463.26949999999</v>
+        <v>83311.9265</v>
       </c>
     </row>
     <row r="18">
@@ -672,13 +672,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>95154</v>
+        <v>92477</v>
       </c>
       <c r="C18" t="n">
-        <v>16574.537</v>
+        <v>16384.389</v>
       </c>
       <c r="D18" t="n">
-        <v>78579.463</v>
+        <v>76092.611</v>
       </c>
     </row>
     <row r="19">
@@ -686,69 +686,57 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>98298</v>
+        <v>1237</v>
       </c>
       <c r="C19" t="n">
-        <v>16188.1545</v>
+        <v>15932.637</v>
       </c>
       <c r="D19" t="n">
-        <v>82109.8455</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
         <v>19</v>
       </c>
-      <c r="B20" t="n">
-        <v>94420</v>
-      </c>
       <c r="C20" t="n">
-        <v>15598.3275</v>
+        <v>15036.9065</v>
       </c>
       <c r="D20" t="n">
-        <v>78821.6725</v>
+        <v>81334.0935</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
         <v>20</v>
       </c>
-      <c r="B21" t="n">
-        <v>92856</v>
-      </c>
       <c r="C21" t="n">
-        <v>14119.9695</v>
+        <v>13330.5025</v>
       </c>
       <c r="D21" t="n">
-        <v>78736.03049999999</v>
+        <v>78578.4975</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
         <v>21</v>
       </c>
-      <c r="B22" t="n">
-        <v>88965</v>
-      </c>
       <c r="C22" t="n">
-        <v>12189.1525</v>
+        <v>11770.8115</v>
       </c>
       <c r="D22" t="n">
-        <v>76775.8475</v>
+        <v>77749.1885</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
         <v>22</v>
       </c>
-      <c r="B23" t="n">
-        <v>42562</v>
-      </c>
       <c r="C23" t="n">
-        <v>9406.733</v>
+        <v>9312.075499999999</v>
       </c>
       <c r="D23" t="n">
-        <v>33155.267</v>
+        <v>74837.92449999999</v>
       </c>
     </row>
     <row r="24">
@@ -756,10 +744,10 @@
         <v>23</v>
       </c>
       <c r="C24" t="n">
-        <v>6502.2755</v>
+        <v>6773.7985</v>
       </c>
       <c r="D24" t="n">
-        <v>67476.7245</v>
+        <v>54075.2015</v>
       </c>
     </row>
     <row r="25">
@@ -767,7 +755,7 @@
         <v>24</v>
       </c>
       <c r="C25" t="n">
-        <v>5603.15</v>
+        <v>5542.130999999999</v>
       </c>
       <c r="D25" t="n">
         <v>14561.85</v>

</xml_diff>

<commit_message>
Deleted, modified, and added files
</commit_message>
<xml_diff>
--- a/actual_energy.xlsx
+++ b/actual_energy.xlsx
@@ -448,13 +448,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>72056</v>
+        <v>90862</v>
       </c>
       <c r="C2" t="n">
-        <v>5516.6335</v>
+        <v>5539.9085</v>
       </c>
       <c r="D2" t="n">
-        <v>66539.3665</v>
+        <v>85322.09149999999</v>
       </c>
     </row>
     <row r="3">
@@ -462,13 +462,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>69308</v>
+        <v>71987</v>
       </c>
       <c r="C3" t="n">
-        <v>5387.312</v>
+        <v>5343.505999999999</v>
       </c>
       <c r="D3" t="n">
-        <v>63920.688</v>
+        <v>66643.49400000001</v>
       </c>
     </row>
     <row r="4">
@@ -476,13 +476,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>65612</v>
+        <v>69101</v>
       </c>
       <c r="C4" t="n">
-        <v>5339.824000000001</v>
+        <v>5250.640500000001</v>
       </c>
       <c r="D4" t="n">
-        <v>60272.176</v>
+        <v>63850.3595</v>
       </c>
     </row>
     <row r="5">
@@ -490,13 +490,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>64269</v>
+        <v>67174</v>
       </c>
       <c r="C5" t="n">
-        <v>5306.819000000001</v>
+        <v>5194.129499999999</v>
       </c>
       <c r="D5" t="n">
-        <v>58962.181</v>
+        <v>61979.8705</v>
       </c>
     </row>
     <row r="6">
@@ -504,13 +504,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>65136</v>
+        <v>67709</v>
       </c>
       <c r="C6" t="n">
-        <v>5338.83</v>
+        <v>5143.397</v>
       </c>
       <c r="D6" t="n">
-        <v>59797.17</v>
+        <v>62565.603</v>
       </c>
     </row>
     <row r="7">
@@ -518,13 +518,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>71065</v>
+        <v>79680</v>
       </c>
       <c r="C7" t="n">
-        <v>5422.714499999999</v>
+        <v>5188.8305</v>
       </c>
       <c r="D7" t="n">
-        <v>65642.2855</v>
+        <v>74491.1695</v>
       </c>
     </row>
     <row r="8">
@@ -532,13 +532,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>70049</v>
+        <v>66217</v>
       </c>
       <c r="C8" t="n">
-        <v>5875.107</v>
+        <v>5628.136500000001</v>
       </c>
       <c r="D8" t="n">
-        <v>64173.893</v>
+        <v>60588.8635</v>
       </c>
     </row>
     <row r="9">
@@ -546,13 +546,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>80484</v>
+        <v>73755</v>
       </c>
       <c r="C9" t="n">
-        <v>7214.4275</v>
+        <v>6549.074000000001</v>
       </c>
       <c r="D9" t="n">
-        <v>73269.57249999999</v>
+        <v>67205.92599999999</v>
       </c>
     </row>
     <row r="10">
@@ -560,13 +560,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>94725</v>
+        <v>82980</v>
       </c>
       <c r="C10" t="n">
-        <v>8467.018</v>
+        <v>7809.641</v>
       </c>
       <c r="D10" t="n">
-        <v>86257.982</v>
+        <v>75170.359</v>
       </c>
     </row>
     <row r="11">
@@ -574,13 +574,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>104123</v>
+        <v>95273</v>
       </c>
       <c r="C11" t="n">
-        <v>13640.6165</v>
+        <v>12977.8705</v>
       </c>
       <c r="D11" t="n">
-        <v>90482.3835</v>
+        <v>82295.1295</v>
       </c>
     </row>
     <row r="12">
@@ -588,13 +588,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>110312</v>
+        <v>97940</v>
       </c>
       <c r="C12" t="n">
-        <v>15763.02</v>
+        <v>14879.494</v>
       </c>
       <c r="D12" t="n">
-        <v>94548.98</v>
+        <v>83060.50599999999</v>
       </c>
     </row>
     <row r="13">
@@ -602,13 +602,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>111321</v>
+        <v>95015</v>
       </c>
       <c r="C13" t="n">
-        <v>15072.0395</v>
+        <v>15334.284</v>
       </c>
       <c r="D13" t="n">
-        <v>96248.9605</v>
+        <v>79680.716</v>
       </c>
     </row>
     <row r="14">
@@ -616,13 +616,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>109259</v>
+        <v>103218</v>
       </c>
       <c r="C14" t="n">
-        <v>15259.6675</v>
+        <v>15538.4565</v>
       </c>
       <c r="D14" t="n">
-        <v>93999.3325</v>
+        <v>87679.5435</v>
       </c>
     </row>
     <row r="15">
@@ -630,13 +630,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>113429</v>
+        <v>100719</v>
       </c>
       <c r="C15" t="n">
-        <v>15815.744</v>
+        <v>15473.9585</v>
       </c>
       <c r="D15" t="n">
-        <v>97613.25599999999</v>
+        <v>85245.04149999999</v>
       </c>
     </row>
     <row r="16">
@@ -644,13 +644,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>114542</v>
+        <v>99562</v>
       </c>
       <c r="C16" t="n">
-        <v>15955.3275</v>
+        <v>15459.3285</v>
       </c>
       <c r="D16" t="n">
-        <v>98586.6725</v>
+        <v>84102.6715</v>
       </c>
     </row>
     <row r="17">
@@ -658,13 +658,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>99426</v>
+        <v>98100</v>
       </c>
       <c r="C17" t="n">
-        <v>16114.0735</v>
+        <v>15733.5675</v>
       </c>
       <c r="D17" t="n">
-        <v>83311.9265</v>
+        <v>82366.4325</v>
       </c>
     </row>
     <row r="18">
@@ -672,13 +672,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>92477</v>
+        <v>94912</v>
       </c>
       <c r="C18" t="n">
-        <v>16384.389</v>
+        <v>15999.228</v>
       </c>
       <c r="D18" t="n">
-        <v>76092.611</v>
+        <v>78912.772</v>
       </c>
     </row>
     <row r="19">
@@ -686,79 +686,97 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>1237</v>
+        <v>93211</v>
       </c>
       <c r="C19" t="n">
-        <v>15932.637</v>
+        <v>15687.07</v>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>77523.92999999999</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
         <v>19</v>
       </c>
+      <c r="B20" t="n">
+        <v>95142</v>
+      </c>
       <c r="C20" t="n">
-        <v>15036.9065</v>
+        <v>15318.933</v>
       </c>
       <c r="D20" t="n">
-        <v>81334.0935</v>
+        <v>79823.067</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
         <v>20</v>
       </c>
+      <c r="B21" t="n">
+        <v>91234</v>
+      </c>
       <c r="C21" t="n">
-        <v>13330.5025</v>
+        <v>13434.6415</v>
       </c>
       <c r="D21" t="n">
-        <v>78578.4975</v>
+        <v>77799.3585</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
         <v>21</v>
       </c>
+      <c r="B22" t="n">
+        <v>88757</v>
+      </c>
       <c r="C22" t="n">
-        <v>11770.8115</v>
+        <v>11609.815</v>
       </c>
       <c r="D22" t="n">
-        <v>77749.1885</v>
+        <v>77147.185</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
         <v>22</v>
       </c>
+      <c r="B23" t="n">
+        <v>85054</v>
+      </c>
       <c r="C23" t="n">
-        <v>9312.075499999999</v>
+        <v>9103.451000000001</v>
       </c>
       <c r="D23" t="n">
-        <v>74837.92449999999</v>
+        <v>75950.549</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
         <v>23</v>
       </c>
+      <c r="B24" t="n">
+        <v>80176</v>
+      </c>
       <c r="C24" t="n">
-        <v>6773.7985</v>
+        <v>6290.4415</v>
       </c>
       <c r="D24" t="n">
-        <v>54075.2015</v>
+        <v>73885.5585</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
         <v>24</v>
       </c>
+      <c r="B25" t="n">
+        <v>76785</v>
+      </c>
       <c r="C25" t="n">
-        <v>5542.130999999999</v>
+        <v>5217.8665</v>
       </c>
       <c r="D25" t="n">
-        <v>14561.85</v>
+        <v>71567.1335</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added, modified, and deleted some files
</commit_message>
<xml_diff>
--- a/actual_energy.xlsx
+++ b/actual_energy.xlsx
@@ -448,13 +448,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>90862</v>
+        <v>65724</v>
       </c>
       <c r="C2" t="n">
-        <v>5539.9085</v>
+        <v>5632.2595</v>
       </c>
       <c r="D2" t="n">
-        <v>85322.09149999999</v>
+        <v>60091.7405</v>
       </c>
     </row>
     <row r="3">
@@ -462,13 +462,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>71987</v>
+        <v>63085</v>
       </c>
       <c r="C3" t="n">
-        <v>5343.505999999999</v>
+        <v>5478.844000000001</v>
       </c>
       <c r="D3" t="n">
-        <v>66643.49400000001</v>
+        <v>57606.156</v>
       </c>
     </row>
     <row r="4">
@@ -476,13 +476,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>69101</v>
+        <v>61258</v>
       </c>
       <c r="C4" t="n">
-        <v>5250.640500000001</v>
+        <v>5431.737499999999</v>
       </c>
       <c r="D4" t="n">
-        <v>63850.3595</v>
+        <v>55826.2625</v>
       </c>
     </row>
     <row r="5">
@@ -490,13 +490,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>67174</v>
+        <v>60272</v>
       </c>
       <c r="C5" t="n">
-        <v>5194.129499999999</v>
+        <v>5351.2935</v>
       </c>
       <c r="D5" t="n">
-        <v>61979.8705</v>
+        <v>54920.7065</v>
       </c>
     </row>
     <row r="6">
@@ -504,13 +504,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>67709</v>
+        <v>63182</v>
       </c>
       <c r="C6" t="n">
-        <v>5143.397</v>
+        <v>5443.7565</v>
       </c>
       <c r="D6" t="n">
-        <v>62565.603</v>
+        <v>57738.2435</v>
       </c>
     </row>
     <row r="7">
@@ -518,13 +518,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>79680</v>
+        <v>67802</v>
       </c>
       <c r="C7" t="n">
-        <v>5188.8305</v>
+        <v>5521.645500000001</v>
       </c>
       <c r="D7" t="n">
-        <v>74491.1695</v>
+        <v>62280.3545</v>
       </c>
     </row>
     <row r="8">
@@ -532,13 +532,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>66217</v>
+        <v>69571</v>
       </c>
       <c r="C8" t="n">
-        <v>5628.136500000001</v>
+        <v>6568.996000000001</v>
       </c>
       <c r="D8" t="n">
-        <v>60588.8635</v>
+        <v>63002.004</v>
       </c>
     </row>
     <row r="9">
@@ -546,13 +546,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>73755</v>
+        <v>81158</v>
       </c>
       <c r="C9" t="n">
-        <v>6549.074000000001</v>
+        <v>7039.0705</v>
       </c>
       <c r="D9" t="n">
-        <v>67205.92599999999</v>
+        <v>74118.9295</v>
       </c>
     </row>
     <row r="10">
@@ -560,13 +560,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>82980</v>
+        <v>98453</v>
       </c>
       <c r="C10" t="n">
-        <v>7809.641</v>
+        <v>8768.984</v>
       </c>
       <c r="D10" t="n">
-        <v>75170.359</v>
+        <v>89684.016</v>
       </c>
     </row>
     <row r="11">
@@ -574,13 +574,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>95273</v>
+        <v>108429</v>
       </c>
       <c r="C11" t="n">
-        <v>12977.8705</v>
+        <v>14287.7385</v>
       </c>
       <c r="D11" t="n">
-        <v>82295.1295</v>
+        <v>94141.26149999999</v>
       </c>
     </row>
     <row r="12">
@@ -588,13 +588,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>97940</v>
+        <v>111739</v>
       </c>
       <c r="C12" t="n">
-        <v>14879.494</v>
+        <v>16203.32</v>
       </c>
       <c r="D12" t="n">
-        <v>83060.50599999999</v>
+        <v>95535.67999999999</v>
       </c>
     </row>
     <row r="13">
@@ -602,13 +602,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>95015</v>
+        <v>113097</v>
       </c>
       <c r="C13" t="n">
-        <v>15334.284</v>
+        <v>16253.0025</v>
       </c>
       <c r="D13" t="n">
-        <v>79680.716</v>
+        <v>96843.9975</v>
       </c>
     </row>
     <row r="14">
@@ -616,13 +616,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>103218</v>
+        <v>112752</v>
       </c>
       <c r="C14" t="n">
-        <v>15538.4565</v>
+        <v>16193.9575</v>
       </c>
       <c r="D14" t="n">
-        <v>87679.5435</v>
+        <v>96558.0425</v>
       </c>
     </row>
     <row r="15">
@@ -630,13 +630,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>100719</v>
+        <v>116975</v>
       </c>
       <c r="C15" t="n">
-        <v>15473.9585</v>
+        <v>16307.025</v>
       </c>
       <c r="D15" t="n">
-        <v>85245.04149999999</v>
+        <v>100667.975</v>
       </c>
     </row>
     <row r="16">
@@ -644,13 +644,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>99562</v>
+        <v>117642</v>
       </c>
       <c r="C16" t="n">
-        <v>15459.3285</v>
+        <v>16253.9055</v>
       </c>
       <c r="D16" t="n">
-        <v>84102.6715</v>
+        <v>101388.0945</v>
       </c>
     </row>
     <row r="17">
@@ -658,13 +658,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>98100</v>
+        <v>96422</v>
       </c>
       <c r="C17" t="n">
-        <v>15733.5675</v>
+        <v>15667.071</v>
       </c>
       <c r="D17" t="n">
-        <v>82366.4325</v>
+        <v>80754.929</v>
       </c>
     </row>
     <row r="18">
@@ -672,24 +672,21 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>94912</v>
+        <v>94648</v>
       </c>
       <c r="C18" t="n">
-        <v>15999.228</v>
+        <v>16597.392</v>
       </c>
       <c r="D18" t="n">
-        <v>78912.772</v>
+        <v>78050.60800000001</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
         <v>18</v>
       </c>
-      <c r="B19" t="n">
-        <v>93211</v>
-      </c>
       <c r="C19" t="n">
-        <v>15687.07</v>
+        <v>16121.5775</v>
       </c>
       <c r="D19" t="n">
         <v>77523.92999999999</v>
@@ -699,11 +696,8 @@
       <c r="A20" t="n">
         <v>19</v>
       </c>
-      <c r="B20" t="n">
-        <v>95142</v>
-      </c>
       <c r="C20" t="n">
-        <v>15318.933</v>
+        <v>15277.878</v>
       </c>
       <c r="D20" t="n">
         <v>79823.067</v>
@@ -713,11 +707,8 @@
       <c r="A21" t="n">
         <v>20</v>
       </c>
-      <c r="B21" t="n">
-        <v>91234</v>
-      </c>
       <c r="C21" t="n">
-        <v>13434.6415</v>
+        <v>13983.214</v>
       </c>
       <c r="D21" t="n">
         <v>77799.3585</v>
@@ -727,11 +718,8 @@
       <c r="A22" t="n">
         <v>21</v>
       </c>
-      <c r="B22" t="n">
-        <v>88757</v>
-      </c>
       <c r="C22" t="n">
-        <v>11609.815</v>
+        <v>12008.9865</v>
       </c>
       <c r="D22" t="n">
         <v>77147.185</v>
@@ -741,11 +729,8 @@
       <c r="A23" t="n">
         <v>22</v>
       </c>
-      <c r="B23" t="n">
-        <v>85054</v>
-      </c>
       <c r="C23" t="n">
-        <v>9103.451000000001</v>
+        <v>9648.002000000002</v>
       </c>
       <c r="D23" t="n">
         <v>75950.549</v>
@@ -755,11 +740,8 @@
       <c r="A24" t="n">
         <v>23</v>
       </c>
-      <c r="B24" t="n">
-        <v>80176</v>
-      </c>
       <c r="C24" t="n">
-        <v>6290.4415</v>
+        <v>6756.816500000001</v>
       </c>
       <c r="D24" t="n">
         <v>73885.5585</v>
@@ -769,11 +751,8 @@
       <c r="A25" t="n">
         <v>24</v>
       </c>
-      <c r="B25" t="n">
-        <v>76785</v>
-      </c>
       <c r="C25" t="n">
-        <v>5217.8665</v>
+        <v>6005.93</v>
       </c>
       <c r="D25" t="n">
         <v>71567.1335</v>

</xml_diff>

<commit_message>
Added, deleted, and modified some files
</commit_message>
<xml_diff>
--- a/actual_energy.xlsx
+++ b/actual_energy.xlsx
@@ -448,13 +448,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>65724</v>
+        <v>73158</v>
       </c>
       <c r="C2" t="n">
-        <v>5632.2595</v>
+        <v>5416.988499999999</v>
       </c>
       <c r="D2" t="n">
-        <v>60091.7405</v>
+        <v>67741.01150000001</v>
       </c>
     </row>
     <row r="3">
@@ -462,13 +462,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>63085</v>
+        <v>69971</v>
       </c>
       <c r="C3" t="n">
-        <v>5478.844000000001</v>
+        <v>5210.142</v>
       </c>
       <c r="D3" t="n">
-        <v>57606.156</v>
+        <v>64760.858</v>
       </c>
     </row>
     <row r="4">
@@ -476,13 +476,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>61258</v>
+        <v>67233</v>
       </c>
       <c r="C4" t="n">
-        <v>5431.737499999999</v>
+        <v>5131.699999999999</v>
       </c>
       <c r="D4" t="n">
-        <v>55826.2625</v>
+        <v>62101.3</v>
       </c>
     </row>
     <row r="5">
@@ -490,13 +490,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>60272</v>
+        <v>66774</v>
       </c>
       <c r="C5" t="n">
-        <v>5351.2935</v>
+        <v>5049.197999999999</v>
       </c>
       <c r="D5" t="n">
-        <v>54920.7065</v>
+        <v>61724.802</v>
       </c>
     </row>
     <row r="6">
@@ -504,13 +504,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>63182</v>
+        <v>68427</v>
       </c>
       <c r="C6" t="n">
-        <v>5443.7565</v>
+        <v>5084.9925</v>
       </c>
       <c r="D6" t="n">
-        <v>57738.2435</v>
+        <v>63342.0075</v>
       </c>
     </row>
     <row r="7">
@@ -518,13 +518,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>67802</v>
+        <v>72833</v>
       </c>
       <c r="C7" t="n">
-        <v>5521.645500000001</v>
+        <v>5380.1055</v>
       </c>
       <c r="D7" t="n">
-        <v>62280.3545</v>
+        <v>67452.89449999999</v>
       </c>
     </row>
     <row r="8">
@@ -532,13 +532,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>69571</v>
+        <v>72858</v>
       </c>
       <c r="C8" t="n">
-        <v>6568.996000000001</v>
+        <v>6413.1515</v>
       </c>
       <c r="D8" t="n">
-        <v>63002.004</v>
+        <v>66444.84849999999</v>
       </c>
     </row>
     <row r="9">
@@ -546,13 +546,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>81158</v>
+        <v>84685</v>
       </c>
       <c r="C9" t="n">
-        <v>7039.0705</v>
+        <v>7207.8405</v>
       </c>
       <c r="D9" t="n">
-        <v>74118.9295</v>
+        <v>77477.15949999999</v>
       </c>
     </row>
     <row r="10">
@@ -560,13 +560,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>98453</v>
+        <v>102552</v>
       </c>
       <c r="C10" t="n">
-        <v>8768.984</v>
+        <v>9489.200000000001</v>
       </c>
       <c r="D10" t="n">
-        <v>89684.016</v>
+        <v>93062.8</v>
       </c>
     </row>
     <row r="11">
@@ -574,13 +574,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>108429</v>
+        <v>112257</v>
       </c>
       <c r="C11" t="n">
-        <v>14287.7385</v>
+        <v>14318.1885</v>
       </c>
       <c r="D11" t="n">
-        <v>94141.26149999999</v>
+        <v>97938.8115</v>
       </c>
     </row>
     <row r="12">
@@ -588,13 +588,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>111739</v>
+        <v>116157</v>
       </c>
       <c r="C12" t="n">
-        <v>16203.32</v>
+        <v>15340.192</v>
       </c>
       <c r="D12" t="n">
-        <v>95535.67999999999</v>
+        <v>100816.808</v>
       </c>
     </row>
     <row r="13">
@@ -602,13 +602,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>113097</v>
+        <v>115181</v>
       </c>
       <c r="C13" t="n">
-        <v>16253.0025</v>
+        <v>15589.8715</v>
       </c>
       <c r="D13" t="n">
-        <v>96843.9975</v>
+        <v>99591.12850000001</v>
       </c>
     </row>
     <row r="14">
@@ -616,13 +616,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>112752</v>
+        <v>118438</v>
       </c>
       <c r="C14" t="n">
-        <v>16193.9575</v>
+        <v>15359.3685</v>
       </c>
       <c r="D14" t="n">
-        <v>96558.0425</v>
+        <v>103078.6315</v>
       </c>
     </row>
     <row r="15">
@@ -630,13 +630,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>116975</v>
+        <v>118968</v>
       </c>
       <c r="C15" t="n">
-        <v>16307.025</v>
+        <v>15511.44</v>
       </c>
       <c r="D15" t="n">
-        <v>100667.975</v>
+        <v>103456.56</v>
       </c>
     </row>
     <row r="16">
@@ -644,13 +644,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>117642</v>
+        <v>121806</v>
       </c>
       <c r="C16" t="n">
-        <v>16253.9055</v>
+        <v>15666.4375</v>
       </c>
       <c r="D16" t="n">
-        <v>101388.0945</v>
+        <v>106139.5625</v>
       </c>
     </row>
     <row r="17">
@@ -658,13 +658,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>96422</v>
+        <v>114966</v>
       </c>
       <c r="C17" t="n">
-        <v>15667.071</v>
+        <v>16125.417</v>
       </c>
       <c r="D17" t="n">
-        <v>80754.929</v>
+        <v>98840.583</v>
       </c>
     </row>
     <row r="18">
@@ -672,13 +672,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>94648</v>
+        <v>15556</v>
       </c>
       <c r="C18" t="n">
-        <v>16597.392</v>
+        <v>16406.873</v>
       </c>
       <c r="D18" t="n">
-        <v>78050.60800000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -686,10 +686,10 @@
         <v>18</v>
       </c>
       <c r="C19" t="n">
-        <v>16121.5775</v>
+        <v>16163.1645</v>
       </c>
       <c r="D19" t="n">
-        <v>77523.92999999999</v>
+        <v>91921.8355</v>
       </c>
     </row>
     <row r="20">
@@ -697,10 +697,10 @@
         <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>15277.878</v>
+        <v>15659.7175</v>
       </c>
       <c r="D20" t="n">
-        <v>79823.067</v>
+        <v>91677.2825</v>
       </c>
     </row>
     <row r="21">
@@ -708,10 +708,10 @@
         <v>20</v>
       </c>
       <c r="C21" t="n">
-        <v>13983.214</v>
+        <v>13764.5865</v>
       </c>
       <c r="D21" t="n">
-        <v>77799.3585</v>
+        <v>78811.4135</v>
       </c>
     </row>
     <row r="22">
@@ -719,10 +719,10 @@
         <v>21</v>
       </c>
       <c r="C22" t="n">
-        <v>12008.9865</v>
+        <v>11506.208</v>
       </c>
       <c r="D22" t="n">
-        <v>77147.185</v>
+        <v>80527.792</v>
       </c>
     </row>
     <row r="23">
@@ -730,10 +730,10 @@
         <v>22</v>
       </c>
       <c r="C23" t="n">
-        <v>9648.002000000002</v>
+        <v>8102.793999999999</v>
       </c>
       <c r="D23" t="n">
-        <v>75950.549</v>
+        <v>59160.206</v>
       </c>
     </row>
     <row r="24">
@@ -741,10 +741,10 @@
         <v>23</v>
       </c>
       <c r="C24" t="n">
-        <v>6756.816500000001</v>
+        <v>6308.112999999999</v>
       </c>
       <c r="D24" t="n">
-        <v>73885.5585</v>
+        <v>65087.887</v>
       </c>
     </row>
     <row r="25">
@@ -752,7 +752,7 @@
         <v>24</v>
       </c>
       <c r="C25" t="n">
-        <v>6005.93</v>
+        <v>5711.482</v>
       </c>
       <c r="D25" t="n">
         <v>71567.1335</v>

</xml_diff>

<commit_message>
Added, deleted, and modified files
</commit_message>
<xml_diff>
--- a/actual_energy.xlsx
+++ b/actual_energy.xlsx
@@ -448,13 +448,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>16686.6685</v>
+        <v>54000</v>
       </c>
       <c r="C2" t="n">
-        <v>5731.74</v>
+        <v>4944.292321154038</v>
       </c>
       <c r="D2" t="n">
-        <v>10954.9285</v>
+        <v>49055.70767884596</v>
       </c>
     </row>
     <row r="3">
@@ -462,13 +462,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>16181.618</v>
+        <v>50801</v>
       </c>
       <c r="C3" t="n">
-        <v>5526.115</v>
+        <v>4887.559847582665</v>
       </c>
       <c r="D3" t="n">
-        <v>10655.503</v>
+        <v>45913.44015241734</v>
       </c>
     </row>
     <row r="4">
@@ -476,13 +476,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>15829.5828</v>
+        <v>48611</v>
       </c>
       <c r="C4" t="n">
-        <v>5390.847</v>
+        <v>4825.545484664752</v>
       </c>
       <c r="D4" t="n">
-        <v>10438.7358</v>
+        <v>43785.45451533525</v>
       </c>
     </row>
     <row r="5">
@@ -490,13 +490,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>15668.5667</v>
+        <v>46724</v>
       </c>
       <c r="C5" t="n">
-        <v>5356.008</v>
+        <v>4794.057447783162</v>
       </c>
       <c r="D5" t="n">
-        <v>10312.5587</v>
+        <v>41929.94255221684</v>
       </c>
     </row>
     <row r="6">
@@ -504,13 +504,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>15742.5741</v>
+        <v>47566</v>
       </c>
       <c r="C6" t="n">
-        <v>5438.279</v>
+        <v>4794.010622970725</v>
       </c>
       <c r="D6" t="n">
-        <v>10304.2951</v>
+        <v>42771.98937702928</v>
       </c>
     </row>
     <row r="7">
@@ -518,13 +518,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>16879.6878</v>
+        <v>48485</v>
       </c>
       <c r="C7" t="n">
-        <v>5565.175</v>
+        <v>4890.506649537315</v>
       </c>
       <c r="D7" t="n">
-        <v>11314.5128</v>
+        <v>43594.49335046268</v>
       </c>
     </row>
     <row r="8">
@@ -532,13 +532,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>17433.7432</v>
+        <v>47871</v>
       </c>
       <c r="C8" t="n">
-        <v>6573.994000000001</v>
+        <v>5267.449152182856</v>
       </c>
       <c r="D8" t="n">
-        <v>10859.7492</v>
+        <v>42603.55084781715</v>
       </c>
     </row>
     <row r="9">
@@ -546,13 +546,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>18994.8993</v>
+        <v>41983</v>
       </c>
       <c r="C9" t="n">
-        <v>7376.026</v>
+        <v>6573.678702600464</v>
       </c>
       <c r="D9" t="n">
-        <v>11618.8733</v>
+        <v>35409.32129739954</v>
       </c>
     </row>
     <row r="10">
@@ -560,13 +560,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>23161.3159</v>
+        <v>65400</v>
       </c>
       <c r="C10" t="n">
-        <v>8830.576999999997</v>
+        <v>8191.789500000001</v>
       </c>
       <c r="D10" t="n">
-        <v>14330.7389</v>
+        <v>57208.2105</v>
       </c>
     </row>
     <row r="11">
@@ -574,13 +574,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>24740.4738</v>
+        <v>73839</v>
       </c>
       <c r="C11" t="n">
-        <v>13925.926</v>
+        <v>14018.138</v>
       </c>
       <c r="D11" t="n">
-        <v>10814.5478</v>
+        <v>59820.862</v>
       </c>
     </row>
     <row r="12">
@@ -588,13 +588,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>25525.5523</v>
+        <v>77636</v>
       </c>
       <c r="C12" t="n">
-        <v>16103.297</v>
+        <v>14986.9245</v>
       </c>
       <c r="D12" t="n">
-        <v>9422.255299999999</v>
+        <v>62649.0755</v>
       </c>
     </row>
     <row r="13">
@@ -602,46 +602,55 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>78566</v>
       </c>
       <c r="C13" t="n">
-        <v>15849.1235</v>
+        <v>14980.626</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>63585.374</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
         <v>13</v>
       </c>
+      <c r="B14" t="n">
+        <v>79318</v>
+      </c>
       <c r="C14" t="n">
-        <v>15935.9585</v>
+        <v>15169.25375</v>
       </c>
       <c r="D14" t="n">
-        <v>96816.04149999999</v>
+        <v>64148.74625</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
         <v>14</v>
       </c>
+      <c r="B15" t="n">
+        <v>83095</v>
+      </c>
       <c r="C15" t="n">
-        <v>15893.2095</v>
+        <v>15666.69225</v>
       </c>
       <c r="D15" t="n">
-        <v>101081.7905</v>
+        <v>67428.30775000001</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
         <v>15</v>
       </c>
+      <c r="B16" t="n">
+        <v>51910</v>
+      </c>
       <c r="C16" t="n">
-        <v>16461.3505</v>
+        <v>15813.73925</v>
       </c>
       <c r="D16" t="n">
-        <v>101180.6495</v>
+        <v>36096.26075</v>
       </c>
     </row>
     <row r="17">
@@ -649,10 +658,10 @@
         <v>16</v>
       </c>
       <c r="C17" t="n">
-        <v>16893.7965</v>
+        <v>16092.652</v>
       </c>
       <c r="D17" t="n">
-        <v>79528.2035</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -660,10 +669,10 @@
         <v>17</v>
       </c>
       <c r="C18" t="n">
-        <v>16943.689</v>
+        <v>16268.66525</v>
       </c>
       <c r="D18" t="n">
-        <v>77704.311</v>
+        <v>1768.269410000001</v>
       </c>
     </row>
     <row r="19">
@@ -671,10 +680,10 @@
         <v>18</v>
       </c>
       <c r="C19" t="n">
-        <v>15829.6355</v>
+        <v>16049.11175</v>
       </c>
       <c r="D19" t="n">
-        <v>66661.442085</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -682,10 +691,10 @@
         <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>15704.7975</v>
+        <v>14955.2725</v>
       </c>
       <c r="D20" t="n">
-        <v>67736.5061</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -693,10 +702,10 @@
         <v>20</v>
       </c>
       <c r="C21" t="n">
-        <v>14246.386</v>
+        <v>13776.544</v>
       </c>
       <c r="D21" t="n">
-        <v>65913.62435500001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -704,10 +713,10 @@
         <v>21</v>
       </c>
       <c r="C22" t="n">
-        <v>11999.0745</v>
+        <v>12164.7975</v>
       </c>
       <c r="D22" t="n">
-        <v>64058.817675</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -715,10 +724,10 @@
         <v>22</v>
       </c>
       <c r="C23" t="n">
-        <v>9654.239000000001</v>
+        <v>9625.974749999999</v>
       </c>
       <c r="D23" t="n">
-        <v>63120.0028</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -726,10 +735,10 @@
         <v>23</v>
       </c>
       <c r="C24" t="n">
-        <v>6915.5555</v>
+        <v>6491.415499999999</v>
       </c>
       <c r="D24" t="n">
-        <v>60502.067025</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -737,10 +746,10 @@
         <v>24</v>
       </c>
       <c r="C25" t="n">
-        <v>5962.4075</v>
+        <v>5924.492750000001</v>
       </c>
       <c r="D25" t="n">
-        <v>23066.7285</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified the requirements.txt file
</commit_message>
<xml_diff>
--- a/actual_energy.xlsx
+++ b/actual_energy.xlsx
@@ -672,68 +672,83 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>55356</v>
+        <v>58430</v>
       </c>
       <c r="C18" t="n">
         <v>16764.4865</v>
       </c>
       <c r="D18" t="n">
-        <v>38591.5135</v>
+        <v>41665.5135</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
         <v>18</v>
       </c>
+      <c r="B19" t="n">
+        <v>56357</v>
+      </c>
       <c r="C19" t="n">
         <v>16629.4945</v>
       </c>
       <c r="D19" t="n">
-        <v>0</v>
+        <v>39727.5055</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
         <v>19</v>
       </c>
+      <c r="B20" t="n">
+        <v>55191</v>
+      </c>
       <c r="C20" t="n">
         <v>16025.2325</v>
       </c>
       <c r="D20" t="n">
-        <v>0</v>
+        <v>39165.7675</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
         <v>20</v>
       </c>
+      <c r="B21" t="n">
+        <v>52357</v>
+      </c>
       <c r="C21" t="n">
         <v>14539.505</v>
       </c>
       <c r="D21" t="n">
-        <v>0</v>
+        <v>37817.495</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
         <v>21</v>
       </c>
+      <c r="B22" t="n">
+        <v>50614</v>
+      </c>
       <c r="C22" t="n">
         <v>12603.773</v>
       </c>
       <c r="D22" t="n">
-        <v>0</v>
+        <v>38010.227</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
         <v>22</v>
       </c>
+      <c r="B23" t="n">
+        <v>47951</v>
+      </c>
       <c r="C23" t="n">
         <v>9665.7935</v>
       </c>
       <c r="D23" t="n">
-        <v>0</v>
+        <v>38285.2065</v>
       </c>
     </row>
     <row r="24">

</xml_diff>

<commit_message>
Added latest DAP file
</commit_message>
<xml_diff>
--- a/actual_energy.xlsx
+++ b/actual_energy.xlsx
@@ -448,13 +448,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>39477</v>
+        <v>33061</v>
       </c>
       <c r="C2" t="n">
-        <v>5801.188</v>
+        <v>5005.48337366473</v>
       </c>
       <c r="D2" t="n">
-        <v>33675.812</v>
+        <v>28055.51662633527</v>
       </c>
     </row>
     <row r="3">
@@ -462,13 +462,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>37915</v>
+        <v>31828</v>
       </c>
       <c r="C3" t="n">
-        <v>5641.719000000001</v>
+        <v>4922.298456099087</v>
       </c>
       <c r="D3" t="n">
-        <v>32273.281</v>
+        <v>26905.70154390091</v>
       </c>
     </row>
     <row r="4">
@@ -476,13 +476,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>36600</v>
+        <v>30574</v>
       </c>
       <c r="C4" t="n">
-        <v>5541.0945</v>
+        <v>4850.625419333438</v>
       </c>
       <c r="D4" t="n">
-        <v>31058.9055</v>
+        <v>25723.37458066656</v>
       </c>
     </row>
     <row r="5">
@@ -490,13 +490,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>35560</v>
+        <v>29643</v>
       </c>
       <c r="C5" t="n">
-        <v>5516.280000000001</v>
+        <v>4797.274898040722</v>
       </c>
       <c r="D5" t="n">
-        <v>30043.72</v>
+        <v>24845.72510195928</v>
       </c>
     </row>
     <row r="6">
@@ -504,13 +504,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>35955</v>
+        <v>29848</v>
       </c>
       <c r="C6" t="n">
-        <v>5497.001</v>
+        <v>4859.095012476347</v>
       </c>
       <c r="D6" t="n">
-        <v>30457.999</v>
+        <v>24988.90498752365</v>
       </c>
     </row>
     <row r="7">
@@ -518,13 +518,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>38201</v>
+        <v>30796</v>
       </c>
       <c r="C7" t="n">
-        <v>5761.397999999999</v>
+        <v>4960.889853826959</v>
       </c>
       <c r="D7" t="n">
-        <v>32439.602</v>
+        <v>25835.11014617304</v>
       </c>
     </row>
     <row r="8">
@@ -532,13 +532,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>39591</v>
+        <v>31613</v>
       </c>
       <c r="C8" t="n">
-        <v>6103.384</v>
+        <v>5211.449593293681</v>
       </c>
       <c r="D8" t="n">
-        <v>33487.616</v>
+        <v>26401.55040670632</v>
       </c>
     </row>
     <row r="9">
@@ -546,13 +546,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>43811</v>
+        <v>34939</v>
       </c>
       <c r="C9" t="n">
-        <v>6908.593</v>
+        <v>6049.649550323782</v>
       </c>
       <c r="D9" t="n">
-        <v>36902.407</v>
+        <v>28889.35044967622</v>
       </c>
     </row>
     <row r="10">
@@ -560,13 +560,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>53945</v>
+        <v>41934</v>
       </c>
       <c r="C10" t="n">
-        <v>8421.428500000002</v>
+        <v>8417.127547097272</v>
       </c>
       <c r="D10" t="n">
-        <v>45523.5715</v>
+        <v>33516.87245290272</v>
       </c>
     </row>
     <row r="11">
@@ -574,13 +574,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>60389</v>
+        <v>43152</v>
       </c>
       <c r="C11" t="n">
-        <v>14998.9355</v>
+        <v>13902.175</v>
       </c>
       <c r="D11" t="n">
-        <v>45390.0645</v>
+        <v>29249.825</v>
       </c>
     </row>
     <row r="12">
@@ -588,13 +588,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>62710</v>
+        <v>44379</v>
       </c>
       <c r="C12" t="n">
-        <v>14970.028</v>
+        <v>15210.828</v>
       </c>
       <c r="D12" t="n">
-        <v>47739.972</v>
+        <v>29168.172</v>
       </c>
     </row>
     <row r="13">
@@ -602,13 +602,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>64109</v>
+        <v>45163</v>
       </c>
       <c r="C13" t="n">
-        <v>15231.207</v>
+        <v>15097.205</v>
       </c>
       <c r="D13" t="n">
-        <v>48877.793</v>
+        <v>30065.795</v>
       </c>
     </row>
     <row r="14">
@@ -616,13 +616,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>64926</v>
+        <v>45347</v>
       </c>
       <c r="C14" t="n">
-        <v>15435.473</v>
+        <v>14468.754</v>
       </c>
       <c r="D14" t="n">
-        <v>49490.527</v>
+        <v>30878.246</v>
       </c>
     </row>
     <row r="15">
@@ -630,24 +630,21 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>62494</v>
+        <v>47292</v>
       </c>
       <c r="C15" t="n">
-        <v>15934.069</v>
+        <v>14615.9345</v>
       </c>
       <c r="D15" t="n">
-        <v>46559.931</v>
+        <v>32676.0655</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
         <v>15</v>
       </c>
-      <c r="B16" t="n">
-        <v>65765</v>
-      </c>
       <c r="C16" t="n">
-        <v>16001.6455</v>
+        <v>15642.9465</v>
       </c>
       <c r="D16" t="n">
         <v>49763.3545</v>
@@ -657,11 +654,8 @@
       <c r="A17" t="n">
         <v>16</v>
       </c>
-      <c r="B17" t="n">
-        <v>45248</v>
-      </c>
       <c r="C17" t="n">
-        <v>16435.614</v>
+        <v>15864.0115</v>
       </c>
       <c r="D17" t="n">
         <v>28812.386</v>
@@ -671,11 +665,8 @@
       <c r="A18" t="n">
         <v>17</v>
       </c>
-      <c r="B18" t="n">
-        <v>17275</v>
-      </c>
       <c r="C18" t="n">
-        <v>17178.1825</v>
+        <v>16275.092</v>
       </c>
       <c r="D18" t="n">
         <v>96.81750000000102</v>
@@ -686,7 +677,7 @@
         <v>18</v>
       </c>
       <c r="C19" t="n">
-        <v>16939.003</v>
+        <v>16265.2175</v>
       </c>
       <c r="D19" t="n">
         <v>39727.5055</v>
@@ -697,7 +688,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>16685.8825</v>
+        <v>15390.046</v>
       </c>
       <c r="D20" t="n">
         <v>39165.7675</v>
@@ -708,7 +699,7 @@
         <v>20</v>
       </c>
       <c r="C21" t="n">
-        <v>15197.4365</v>
+        <v>13874.261</v>
       </c>
       <c r="D21" t="n">
         <v>37817.495</v>
@@ -719,7 +710,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="n">
-        <v>13342.395</v>
+        <v>11951.5345</v>
       </c>
       <c r="D22" t="n">
         <v>38010.227</v>
@@ -730,7 +721,7 @@
         <v>22</v>
       </c>
       <c r="C23" t="n">
-        <v>9716.890500000001</v>
+        <v>9041.0965</v>
       </c>
       <c r="D23" t="n">
         <v>38285.2065</v>
@@ -741,7 +732,7 @@
         <v>23</v>
       </c>
       <c r="C24" t="n">
-        <v>6391.799999999999</v>
+        <v>6150.5125</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
@@ -752,7 +743,7 @@
         <v>24</v>
       </c>
       <c r="C25" t="n">
-        <v>5848.197</v>
+        <v>5731.305</v>
       </c>
       <c r="D25" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Brought back weather data
</commit_message>
<xml_diff>
--- a/actual_energy.xlsx
+++ b/actual_energy.xlsx
@@ -560,13 +560,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>25946</v>
+        <v>41595</v>
       </c>
       <c r="C10" t="n">
         <v>8421.428500000002</v>
       </c>
       <c r="D10" t="n">
-        <v>17524.5715</v>
+        <v>33173.5715</v>
       </c>
     </row>
     <row r="11">

</xml_diff>

<commit_message>
Modified MORE Trading Node's file path
</commit_message>
<xml_diff>
--- a/actual_energy.xlsx
+++ b/actual_energy.xlsx
@@ -448,13 +448,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>33975</v>
+        <v>36728</v>
       </c>
       <c r="C2" t="n">
-        <v>5801.188</v>
+        <v>5799.800999999999</v>
       </c>
       <c r="D2" t="n">
-        <v>28173.812</v>
+        <v>30928.199</v>
       </c>
     </row>
     <row r="3">
@@ -462,13 +462,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>32265</v>
+        <v>35269</v>
       </c>
       <c r="C3" t="n">
-        <v>5641.719000000001</v>
+        <v>5649.136500000001</v>
       </c>
       <c r="D3" t="n">
-        <v>26623.281</v>
+        <v>29619.8635</v>
       </c>
     </row>
     <row r="4">
@@ -476,13 +476,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>31121</v>
+        <v>33348</v>
       </c>
       <c r="C4" t="n">
-        <v>5541.0945</v>
+        <v>5554.8325</v>
       </c>
       <c r="D4" t="n">
-        <v>25579.9055</v>
+        <v>27793.1675</v>
       </c>
     </row>
     <row r="5">
@@ -490,13 +490,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>30363</v>
+        <v>31700</v>
       </c>
       <c r="C5" t="n">
-        <v>5516.280000000001</v>
+        <v>5481.98</v>
       </c>
       <c r="D5" t="n">
-        <v>24846.72</v>
+        <v>26218.02</v>
       </c>
     </row>
     <row r="6">
@@ -504,13 +504,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>32040</v>
+        <v>30762</v>
       </c>
       <c r="C6" t="n">
-        <v>5497.001</v>
+        <v>5456.8815</v>
       </c>
       <c r="D6" t="n">
-        <v>26542.999</v>
+        <v>25305.1185</v>
       </c>
     </row>
     <row r="7">
@@ -518,13 +518,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>32872</v>
+        <v>30953</v>
       </c>
       <c r="C7" t="n">
-        <v>5761.397999999999</v>
+        <v>5512.395</v>
       </c>
       <c r="D7" t="n">
-        <v>27110.602</v>
+        <v>25440.605</v>
       </c>
     </row>
     <row r="8">
@@ -532,13 +532,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>33186</v>
+        <v>31330</v>
       </c>
       <c r="C8" t="n">
-        <v>6103.384</v>
+        <v>5765.477227722772</v>
       </c>
       <c r="D8" t="n">
-        <v>27082.616</v>
+        <v>25564.52277227723</v>
       </c>
     </row>
     <row r="9">
@@ -546,13 +546,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>35580</v>
+        <v>32595</v>
       </c>
       <c r="C9" t="n">
-        <v>6908.593</v>
+        <v>6519.4465</v>
       </c>
       <c r="D9" t="n">
-        <v>28671.407</v>
+        <v>26075.5535</v>
       </c>
     </row>
     <row r="10">
@@ -560,13 +560,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>41595</v>
+        <v>36208</v>
       </c>
       <c r="C10" t="n">
-        <v>8421.428500000002</v>
+        <v>7901.5895</v>
       </c>
       <c r="D10" t="n">
-        <v>33173.5715</v>
+        <v>28306.4105</v>
       </c>
     </row>
     <row r="11">
@@ -574,13 +574,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>45256</v>
+        <v>39069</v>
       </c>
       <c r="C11" t="n">
-        <v>14998.9355</v>
+        <v>13052.0005</v>
       </c>
       <c r="D11" t="n">
-        <v>30257.0645</v>
+        <v>26016.9995</v>
       </c>
     </row>
     <row r="12">
@@ -588,13 +588,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>46730</v>
+        <v>39884</v>
       </c>
       <c r="C12" t="n">
-        <v>14970.028</v>
+        <v>14886.7985</v>
       </c>
       <c r="D12" t="n">
-        <v>31759.972</v>
+        <v>24997.2015</v>
       </c>
     </row>
     <row r="13">
@@ -602,13 +602,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>46144</v>
+        <v>39218</v>
       </c>
       <c r="C13" t="n">
-        <v>15231.207</v>
+        <v>14810.005</v>
       </c>
       <c r="D13" t="n">
-        <v>30912.793</v>
+        <v>24407.995</v>
       </c>
     </row>
     <row r="14">
@@ -616,13 +616,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>45993</v>
+        <v>38683</v>
       </c>
       <c r="C14" t="n">
-        <v>15435.473</v>
+        <v>14699.3385</v>
       </c>
       <c r="D14" t="n">
-        <v>30557.527</v>
+        <v>23983.6615</v>
       </c>
     </row>
     <row r="15">
@@ -630,57 +630,69 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>30946</v>
+        <v>40878</v>
       </c>
       <c r="C15" t="n">
-        <v>15934.069</v>
+        <v>15357.636</v>
       </c>
       <c r="D15" t="n">
-        <v>15011.931</v>
+        <v>25520.364</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
         <v>15</v>
       </c>
+      <c r="B16" t="n">
+        <v>41508</v>
+      </c>
       <c r="C16" t="n">
-        <v>16001.6455</v>
+        <v>15432.207</v>
       </c>
       <c r="D16" t="n">
-        <v>49763.3545</v>
+        <v>26075.793</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
         <v>16</v>
       </c>
+      <c r="B17" t="n">
+        <v>40766</v>
+      </c>
       <c r="C17" t="n">
-        <v>16435.614</v>
+        <v>15338.9075</v>
       </c>
       <c r="D17" t="n">
-        <v>28812.386</v>
+        <v>25427.0925</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
         <v>17</v>
       </c>
+      <c r="B18" t="n">
+        <v>38994</v>
+      </c>
       <c r="C18" t="n">
-        <v>17178.1825</v>
+        <v>15792.80217625723</v>
       </c>
       <c r="D18" t="n">
-        <v>96.81750000000102</v>
+        <v>23201.19782374277</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
         <v>18</v>
       </c>
+      <c r="B19" t="n">
+        <v>36246</v>
+      </c>
       <c r="C19" t="n">
-        <v>16939.003</v>
+        <v>15557.50171551809</v>
       </c>
       <c r="D19" t="n">
-        <v>39727.5055</v>
+        <v>20688.49828448191</v>
       </c>
     </row>
     <row r="20">
@@ -688,7 +700,7 @@
         <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>16685.8825</v>
+        <v>15152.49877462994</v>
       </c>
       <c r="D20" t="n">
         <v>39165.7675</v>
@@ -699,7 +711,7 @@
         <v>20</v>
       </c>
       <c r="C21" t="n">
-        <v>15197.4365</v>
+        <v>13812.90902852661</v>
       </c>
       <c r="D21" t="n">
         <v>37817.495</v>
@@ -710,7 +722,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="n">
-        <v>13342.395</v>
+        <v>12007.84432898735</v>
       </c>
       <c r="D22" t="n">
         <v>38010.227</v>
@@ -721,7 +733,7 @@
         <v>22</v>
       </c>
       <c r="C23" t="n">
-        <v>9716.890500000001</v>
+        <v>9523.143</v>
       </c>
       <c r="D23" t="n">
         <v>38285.2065</v>
@@ -732,7 +744,7 @@
         <v>23</v>
       </c>
       <c r="C24" t="n">
-        <v>6391.799999999999</v>
+        <v>6375.7855</v>
       </c>
       <c r="D24" t="n">
         <v>0</v>
@@ -743,7 +755,7 @@
         <v>24</v>
       </c>
       <c r="C25" t="n">
-        <v>5848.197</v>
+        <v>5494.996500000001</v>
       </c>
       <c r="D25" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Changed the total bcq nomination file
</commit_message>
<xml_diff>
--- a/actual_energy.xlsx
+++ b/actual_energy.xlsx
@@ -699,11 +699,14 @@
       <c r="A20" t="n">
         <v>19</v>
       </c>
+      <c r="B20" t="n">
+        <v>15680</v>
+      </c>
       <c r="C20" t="n">
         <v>15152.49877462994</v>
       </c>
       <c r="D20" t="n">
-        <v>39165.7675</v>
+        <v>527.5012253700606</v>
       </c>
     </row>
     <row r="21">

</xml_diff>

<commit_message>
Changed actual energy file
</commit_message>
<xml_diff>
--- a/actual_energy.xlsx
+++ b/actual_energy.xlsx
@@ -448,13 +448,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>36728</v>
+        <v>79488</v>
       </c>
       <c r="C2" t="n">
-        <v>5799.800999999999</v>
+        <v>5597.0385765805</v>
       </c>
       <c r="D2" t="n">
-        <v>30928.199</v>
+        <v>73890.9614234195</v>
       </c>
     </row>
     <row r="3">
@@ -462,13 +462,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>35269</v>
+        <v>75184</v>
       </c>
       <c r="C3" t="n">
-        <v>5649.136500000001</v>
+        <v>5427.810091879</v>
       </c>
       <c r="D3" t="n">
-        <v>29619.8635</v>
+        <v>69756.189908121</v>
       </c>
     </row>
     <row r="4">
@@ -476,13 +476,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>33348</v>
+        <v>71544</v>
       </c>
       <c r="C4" t="n">
-        <v>5554.8325</v>
+        <v>5378.673491737501</v>
       </c>
       <c r="D4" t="n">
-        <v>27793.1675</v>
+        <v>66165.3265082625</v>
       </c>
     </row>
     <row r="5">
@@ -490,13 +490,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>31700</v>
+        <v>69610</v>
       </c>
       <c r="C5" t="n">
-        <v>5481.98</v>
+        <v>5348.731399226001</v>
       </c>
       <c r="D5" t="n">
-        <v>26218.02</v>
+        <v>64261.268600774</v>
       </c>
     </row>
     <row r="6">
@@ -504,13 +504,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>30762</v>
+        <v>70806</v>
       </c>
       <c r="C6" t="n">
-        <v>5456.8815</v>
+        <v>5372.321170922</v>
       </c>
       <c r="D6" t="n">
-        <v>25305.1185</v>
+        <v>65433.678829078</v>
       </c>
     </row>
     <row r="7">
@@ -518,13 +518,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>30953</v>
+        <v>73348</v>
       </c>
       <c r="C7" t="n">
-        <v>5512.395</v>
+        <v>5496.759895401</v>
       </c>
       <c r="D7" t="n">
-        <v>25440.605</v>
+        <v>67851.240104599</v>
       </c>
     </row>
     <row r="8">
@@ -532,13 +532,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>31330</v>
+        <v>78137</v>
       </c>
       <c r="C8" t="n">
-        <v>5765.477227722772</v>
+        <v>6441.069913339</v>
       </c>
       <c r="D8" t="n">
-        <v>25564.52277227723</v>
+        <v>71695.930086661</v>
       </c>
     </row>
     <row r="9">
@@ -546,13 +546,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>32595</v>
+        <v>80939</v>
       </c>
       <c r="C9" t="n">
-        <v>6519.4465</v>
+        <v>7184.668538918501</v>
       </c>
       <c r="D9" t="n">
-        <v>26075.5535</v>
+        <v>73754.3314610815</v>
       </c>
     </row>
     <row r="10">
@@ -560,13 +560,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>36208</v>
+        <v>103039</v>
       </c>
       <c r="C10" t="n">
-        <v>7901.5895</v>
+        <v>8465.353500000001</v>
       </c>
       <c r="D10" t="n">
-        <v>28306.4105</v>
+        <v>94573.6465</v>
       </c>
     </row>
     <row r="11">
@@ -574,13 +574,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>39069</v>
+        <v>114408</v>
       </c>
       <c r="C11" t="n">
-        <v>13052.0005</v>
+        <v>14333.5385</v>
       </c>
       <c r="D11" t="n">
-        <v>26016.9995</v>
+        <v>100074.4615</v>
       </c>
     </row>
     <row r="12">
@@ -588,125 +588,101 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>39884</v>
+        <v>96449.10000000001</v>
       </c>
       <c r="C12" t="n">
-        <v>14886.7985</v>
+        <v>15915.495</v>
       </c>
       <c r="D12" t="n">
-        <v>24997.2015</v>
+        <v>80533.60500000001</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
         <v>12</v>
       </c>
-      <c r="B13" t="n">
-        <v>39218</v>
-      </c>
       <c r="C13" t="n">
-        <v>14810.005</v>
+        <v>15771.6165</v>
       </c>
       <c r="D13" t="n">
-        <v>24407.995</v>
+        <v>103987.3835</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
         <v>13</v>
       </c>
-      <c r="B14" t="n">
-        <v>38683</v>
-      </c>
       <c r="C14" t="n">
-        <v>14699.3385</v>
+        <v>15824.06</v>
       </c>
       <c r="D14" t="n">
-        <v>23983.6615</v>
+        <v>76684.94</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
         <v>14</v>
       </c>
-      <c r="B15" t="n">
-        <v>40878</v>
-      </c>
       <c r="C15" t="n">
-        <v>15357.636</v>
+        <v>15963.6205</v>
       </c>
       <c r="D15" t="n">
-        <v>25520.364</v>
+        <v>103417.3795</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
         <v>15</v>
       </c>
-      <c r="B16" t="n">
-        <v>41508</v>
-      </c>
       <c r="C16" t="n">
-        <v>15432.207</v>
+        <v>16132.936</v>
       </c>
       <c r="D16" t="n">
-        <v>26075.793</v>
+        <v>110937.064</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
         <v>16</v>
       </c>
-      <c r="B17" t="n">
-        <v>40766</v>
-      </c>
       <c r="C17" t="n">
-        <v>15338.9075</v>
+        <v>16102.835</v>
       </c>
       <c r="D17" t="n">
-        <v>25427.0925</v>
+        <v>87260.16500000001</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
         <v>17</v>
       </c>
-      <c r="B18" t="n">
-        <v>38994</v>
-      </c>
       <c r="C18" t="n">
-        <v>15792.80217625723</v>
+        <v>16787.6375</v>
       </c>
       <c r="D18" t="n">
-        <v>23201.19782374277</v>
+        <v>81550.3625</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
         <v>18</v>
       </c>
-      <c r="B19" t="n">
-        <v>39323</v>
-      </c>
       <c r="C19" t="n">
-        <v>15557.50171551809</v>
+        <v>16403.816</v>
       </c>
       <c r="D19" t="n">
-        <v>23765.49828448191</v>
+        <v>75216.18400000001</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
         <v>19</v>
       </c>
-      <c r="B20" t="n">
-        <v>41039</v>
-      </c>
       <c r="C20" t="n">
-        <v>15152.49877462994</v>
+        <v>16006.496</v>
       </c>
       <c r="D20" t="n">
-        <v>25886.50122537006</v>
+        <v>71081.504</v>
       </c>
     </row>
     <row r="21">
@@ -714,10 +690,10 @@
         <v>20</v>
       </c>
       <c r="C21" t="n">
-        <v>13812.90902852661</v>
+        <v>14046.071</v>
       </c>
       <c r="D21" t="n">
-        <v>37817.495</v>
+        <v>69127.929</v>
       </c>
     </row>
     <row r="22">
@@ -725,10 +701,10 @@
         <v>21</v>
       </c>
       <c r="C22" t="n">
-        <v>12007.84432898735</v>
+        <v>11183.005</v>
       </c>
       <c r="D22" t="n">
-        <v>38010.227</v>
+        <v>68523.995</v>
       </c>
     </row>
     <row r="23">
@@ -736,10 +712,10 @@
         <v>22</v>
       </c>
       <c r="C23" t="n">
-        <v>9523.143</v>
+        <v>9240.505000000001</v>
       </c>
       <c r="D23" t="n">
-        <v>38285.2065</v>
+        <v>66852.495</v>
       </c>
     </row>
     <row r="24">
@@ -747,10 +723,10 @@
         <v>23</v>
       </c>
       <c r="C24" t="n">
-        <v>6375.7855</v>
+        <v>6857.7675</v>
       </c>
       <c r="D24" t="n">
-        <v>0</v>
+        <v>33754.2325</v>
       </c>
     </row>
     <row r="25">
@@ -758,7 +734,7 @@
         <v>24</v>
       </c>
       <c r="C25" t="n">
-        <v>5494.996500000001</v>
+        <v>6096.6435</v>
       </c>
       <c r="D25" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Changed contestable energy file
</commit_message>
<xml_diff>
--- a/actual_energy.xlsx
+++ b/actual_energy.xlsx
@@ -448,13 +448,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>79488</v>
+        <v>36728</v>
       </c>
       <c r="C2" t="n">
-        <v>5597.0385765805</v>
+        <v>5799.800999999999</v>
       </c>
       <c r="D2" t="n">
-        <v>73890.9614234195</v>
+        <v>30928.199</v>
       </c>
     </row>
     <row r="3">
@@ -462,13 +462,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>75184</v>
+        <v>35269</v>
       </c>
       <c r="C3" t="n">
-        <v>5427.810091879</v>
+        <v>5649.136500000001</v>
       </c>
       <c r="D3" t="n">
-        <v>69756.189908121</v>
+        <v>29619.8635</v>
       </c>
     </row>
     <row r="4">
@@ -476,13 +476,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>71544</v>
+        <v>33348</v>
       </c>
       <c r="C4" t="n">
-        <v>5378.673491737501</v>
+        <v>5554.8325</v>
       </c>
       <c r="D4" t="n">
-        <v>66165.3265082625</v>
+        <v>27793.1675</v>
       </c>
     </row>
     <row r="5">
@@ -490,13 +490,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>69610</v>
+        <v>31700</v>
       </c>
       <c r="C5" t="n">
-        <v>5348.731399226001</v>
+        <v>5481.98</v>
       </c>
       <c r="D5" t="n">
-        <v>64261.268600774</v>
+        <v>26218.02</v>
       </c>
     </row>
     <row r="6">
@@ -504,13 +504,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>70806</v>
+        <v>30762</v>
       </c>
       <c r="C6" t="n">
-        <v>5372.321170922</v>
+        <v>5456.8815</v>
       </c>
       <c r="D6" t="n">
-        <v>65433.678829078</v>
+        <v>25305.1185</v>
       </c>
     </row>
     <row r="7">
@@ -518,13 +518,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>73348</v>
+        <v>30953</v>
       </c>
       <c r="C7" t="n">
-        <v>5496.759895401</v>
+        <v>5512.395</v>
       </c>
       <c r="D7" t="n">
-        <v>67851.240104599</v>
+        <v>25440.605</v>
       </c>
     </row>
     <row r="8">
@@ -532,13 +532,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>78137</v>
+        <v>31330</v>
       </c>
       <c r="C8" t="n">
-        <v>6441.069913339</v>
+        <v>5765.477227722772</v>
       </c>
       <c r="D8" t="n">
-        <v>71695.930086661</v>
+        <v>25564.52277227723</v>
       </c>
     </row>
     <row r="9">
@@ -546,13 +546,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>80939</v>
+        <v>32595</v>
       </c>
       <c r="C9" t="n">
-        <v>7184.668538918501</v>
+        <v>6519.4465</v>
       </c>
       <c r="D9" t="n">
-        <v>73754.3314610815</v>
+        <v>26075.5535</v>
       </c>
     </row>
     <row r="10">
@@ -560,13 +560,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>103039</v>
+        <v>36208</v>
       </c>
       <c r="C10" t="n">
-        <v>8465.353500000001</v>
+        <v>7901.5895</v>
       </c>
       <c r="D10" t="n">
-        <v>94573.6465</v>
+        <v>28306.4105</v>
       </c>
     </row>
     <row r="11">
@@ -574,13 +574,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>114408</v>
+        <v>39069</v>
       </c>
       <c r="C11" t="n">
-        <v>14333.5385</v>
+        <v>13052.0005</v>
       </c>
       <c r="D11" t="n">
-        <v>100074.4615</v>
+        <v>26016.9995</v>
       </c>
     </row>
     <row r="12">
@@ -588,112 +588,139 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>96449.10000000001</v>
+        <v>39884</v>
       </c>
       <c r="C12" t="n">
-        <v>15915.495</v>
+        <v>14886.7985</v>
       </c>
       <c r="D12" t="n">
-        <v>80533.60500000001</v>
+        <v>24997.2015</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
         <v>12</v>
       </c>
+      <c r="B13" t="n">
+        <v>39218</v>
+      </c>
       <c r="C13" t="n">
-        <v>15771.6165</v>
+        <v>14810.005</v>
       </c>
       <c r="D13" t="n">
-        <v>103987.3835</v>
+        <v>24407.995</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
         <v>13</v>
       </c>
+      <c r="B14" t="n">
+        <v>38683</v>
+      </c>
       <c r="C14" t="n">
-        <v>15824.06</v>
+        <v>14699.3385</v>
       </c>
       <c r="D14" t="n">
-        <v>76684.94</v>
+        <v>23983.6615</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
         <v>14</v>
       </c>
+      <c r="B15" t="n">
+        <v>40878</v>
+      </c>
       <c r="C15" t="n">
-        <v>15963.6205</v>
+        <v>15357.636</v>
       </c>
       <c r="D15" t="n">
-        <v>103417.3795</v>
+        <v>25520.364</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
         <v>15</v>
       </c>
+      <c r="B16" t="n">
+        <v>41508</v>
+      </c>
       <c r="C16" t="n">
-        <v>16132.936</v>
+        <v>15432.207</v>
       </c>
       <c r="D16" t="n">
-        <v>110937.064</v>
+        <v>26075.793</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
         <v>16</v>
       </c>
+      <c r="B17" t="n">
+        <v>40766</v>
+      </c>
       <c r="C17" t="n">
-        <v>16102.835</v>
+        <v>15338.9075</v>
       </c>
       <c r="D17" t="n">
-        <v>87260.16500000001</v>
+        <v>25427.0925</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
         <v>17</v>
       </c>
+      <c r="B18" t="n">
+        <v>38994</v>
+      </c>
       <c r="C18" t="n">
-        <v>16787.6375</v>
+        <v>15792.80217625723</v>
       </c>
       <c r="D18" t="n">
-        <v>81550.3625</v>
+        <v>23201.19782374277</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
         <v>18</v>
       </c>
+      <c r="B19" t="n">
+        <v>39323</v>
+      </c>
       <c r="C19" t="n">
-        <v>16403.816</v>
+        <v>15557.50171551809</v>
       </c>
       <c r="D19" t="n">
-        <v>75216.18400000001</v>
+        <v>23765.49828448191</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
         <v>19</v>
       </c>
+      <c r="B20" t="n">
+        <v>41039</v>
+      </c>
       <c r="C20" t="n">
-        <v>16006.496</v>
+        <v>15152.49877462994</v>
       </c>
       <c r="D20" t="n">
-        <v>71081.504</v>
+        <v>25886.50122537006</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
         <v>20</v>
       </c>
+      <c r="B21" t="n">
+        <v>15333</v>
+      </c>
       <c r="C21" t="n">
-        <v>14046.071</v>
+        <v>13812.90902852661</v>
       </c>
       <c r="D21" t="n">
-        <v>69127.929</v>
+        <v>1520.09097147339</v>
       </c>
     </row>
     <row r="22">
@@ -701,7 +728,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="n">
-        <v>11183.005</v>
+        <v>12007.84432898735</v>
       </c>
       <c r="D22" t="n">
         <v>68523.995</v>
@@ -712,7 +739,7 @@
         <v>22</v>
       </c>
       <c r="C23" t="n">
-        <v>9240.505000000001</v>
+        <v>9523.143</v>
       </c>
       <c r="D23" t="n">
         <v>66852.495</v>
@@ -723,7 +750,7 @@
         <v>23</v>
       </c>
       <c r="C24" t="n">
-        <v>6857.7675</v>
+        <v>6375.7855</v>
       </c>
       <c r="D24" t="n">
         <v>33754.2325</v>
@@ -734,7 +761,7 @@
         <v>24</v>
       </c>
       <c r="C25" t="n">
-        <v>6096.6435</v>
+        <v>5494.996500000001</v>
       </c>
       <c r="D25" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Changed the actual energy file
</commit_message>
<xml_diff>
--- a/actual_energy.xlsx
+++ b/actual_energy.xlsx
@@ -448,13 +448,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>36728</v>
+        <v>79488</v>
       </c>
       <c r="C2" t="n">
-        <v>5799.800999999999</v>
+        <v>5597.0385765805</v>
       </c>
       <c r="D2" t="n">
-        <v>30928.199</v>
+        <v>73890.9614234195</v>
       </c>
     </row>
     <row r="3">
@@ -462,13 +462,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>35269</v>
+        <v>75184</v>
       </c>
       <c r="C3" t="n">
-        <v>5649.136500000001</v>
+        <v>5427.810091879</v>
       </c>
       <c r="D3" t="n">
-        <v>29619.8635</v>
+        <v>69756.189908121</v>
       </c>
     </row>
     <row r="4">
@@ -476,13 +476,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>33348</v>
+        <v>71544</v>
       </c>
       <c r="C4" t="n">
-        <v>5554.8325</v>
+        <v>5378.673491737501</v>
       </c>
       <c r="D4" t="n">
-        <v>27793.1675</v>
+        <v>66165.3265082625</v>
       </c>
     </row>
     <row r="5">
@@ -490,13 +490,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>31700</v>
+        <v>69610</v>
       </c>
       <c r="C5" t="n">
-        <v>5481.98</v>
+        <v>5348.731399226001</v>
       </c>
       <c r="D5" t="n">
-        <v>26218.02</v>
+        <v>64261.268600774</v>
       </c>
     </row>
     <row r="6">
@@ -504,13 +504,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>30762</v>
+        <v>70806</v>
       </c>
       <c r="C6" t="n">
-        <v>5456.8815</v>
+        <v>5372.321170922</v>
       </c>
       <c r="D6" t="n">
-        <v>25305.1185</v>
+        <v>65433.678829078</v>
       </c>
     </row>
     <row r="7">
@@ -518,13 +518,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>30953</v>
+        <v>73348</v>
       </c>
       <c r="C7" t="n">
-        <v>5512.395</v>
+        <v>5496.759895401</v>
       </c>
       <c r="D7" t="n">
-        <v>25440.605</v>
+        <v>67851.240104599</v>
       </c>
     </row>
     <row r="8">
@@ -532,13 +532,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>31330</v>
+        <v>78137</v>
       </c>
       <c r="C8" t="n">
-        <v>5765.477227722772</v>
+        <v>6441.069913339</v>
       </c>
       <c r="D8" t="n">
-        <v>25564.52277227723</v>
+        <v>71695.930086661</v>
       </c>
     </row>
     <row r="9">
@@ -546,13 +546,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>32595</v>
+        <v>80939</v>
       </c>
       <c r="C9" t="n">
-        <v>6519.4465</v>
+        <v>7184.668538918501</v>
       </c>
       <c r="D9" t="n">
-        <v>26075.5535</v>
+        <v>73754.3314610815</v>
       </c>
     </row>
     <row r="10">
@@ -560,13 +560,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>36208</v>
+        <v>103039</v>
       </c>
       <c r="C10" t="n">
-        <v>7901.5895</v>
+        <v>8465.353500000001</v>
       </c>
       <c r="D10" t="n">
-        <v>28306.4105</v>
+        <v>94573.6465</v>
       </c>
     </row>
     <row r="11">
@@ -574,13 +574,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>39069</v>
+        <v>114408</v>
       </c>
       <c r="C11" t="n">
-        <v>13052.0005</v>
+        <v>14333.5385</v>
       </c>
       <c r="D11" t="n">
-        <v>26016.9995</v>
+        <v>100074.4615</v>
       </c>
     </row>
     <row r="12">
@@ -588,139 +588,112 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>39884</v>
+        <v>96449.10000000001</v>
       </c>
       <c r="C12" t="n">
-        <v>14886.7985</v>
+        <v>15915.495</v>
       </c>
       <c r="D12" t="n">
-        <v>24997.2015</v>
+        <v>80533.60500000001</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
         <v>12</v>
       </c>
-      <c r="B13" t="n">
-        <v>39218</v>
-      </c>
       <c r="C13" t="n">
-        <v>14810.005</v>
+        <v>15771.6165</v>
       </c>
       <c r="D13" t="n">
-        <v>24407.995</v>
+        <v>103987.3835</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
         <v>13</v>
       </c>
-      <c r="B14" t="n">
-        <v>38683</v>
-      </c>
       <c r="C14" t="n">
-        <v>14699.3385</v>
+        <v>15824.06</v>
       </c>
       <c r="D14" t="n">
-        <v>23983.6615</v>
+        <v>76684.94</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
         <v>14</v>
       </c>
-      <c r="B15" t="n">
-        <v>40878</v>
-      </c>
       <c r="C15" t="n">
-        <v>15357.636</v>
+        <v>15963.6205</v>
       </c>
       <c r="D15" t="n">
-        <v>25520.364</v>
+        <v>103417.3795</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
         <v>15</v>
       </c>
-      <c r="B16" t="n">
-        <v>41508</v>
-      </c>
       <c r="C16" t="n">
-        <v>15432.207</v>
+        <v>16132.936</v>
       </c>
       <c r="D16" t="n">
-        <v>26075.793</v>
+        <v>110937.064</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
         <v>16</v>
       </c>
-      <c r="B17" t="n">
-        <v>40766</v>
-      </c>
       <c r="C17" t="n">
-        <v>15338.9075</v>
+        <v>16102.835</v>
       </c>
       <c r="D17" t="n">
-        <v>25427.0925</v>
+        <v>87260.16500000001</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
         <v>17</v>
       </c>
-      <c r="B18" t="n">
-        <v>38994</v>
-      </c>
       <c r="C18" t="n">
-        <v>15792.80217625723</v>
+        <v>16787.6375</v>
       </c>
       <c r="D18" t="n">
-        <v>23201.19782374277</v>
+        <v>81550.3625</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
         <v>18</v>
       </c>
-      <c r="B19" t="n">
-        <v>39323</v>
-      </c>
       <c r="C19" t="n">
-        <v>15557.50171551809</v>
+        <v>16403.816</v>
       </c>
       <c r="D19" t="n">
-        <v>23765.49828448191</v>
+        <v>75216.18400000001</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
         <v>19</v>
       </c>
-      <c r="B20" t="n">
-        <v>41039</v>
-      </c>
       <c r="C20" t="n">
-        <v>15152.49877462994</v>
+        <v>16006.496</v>
       </c>
       <c r="D20" t="n">
-        <v>25886.50122537006</v>
+        <v>71081.504</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
         <v>20</v>
       </c>
-      <c r="B21" t="n">
-        <v>15333</v>
-      </c>
       <c r="C21" t="n">
-        <v>13812.90902852661</v>
+        <v>14046.071</v>
       </c>
       <c r="D21" t="n">
-        <v>1520.09097147339</v>
+        <v>69127.929</v>
       </c>
     </row>
     <row r="22">
@@ -728,7 +701,7 @@
         <v>21</v>
       </c>
       <c r="C22" t="n">
-        <v>12007.84432898735</v>
+        <v>11183.005</v>
       </c>
       <c r="D22" t="n">
         <v>68523.995</v>
@@ -739,7 +712,7 @@
         <v>22</v>
       </c>
       <c r="C23" t="n">
-        <v>9523.143</v>
+        <v>9240.505000000001</v>
       </c>
       <c r="D23" t="n">
         <v>66852.495</v>
@@ -750,7 +723,7 @@
         <v>23</v>
       </c>
       <c r="C24" t="n">
-        <v>6375.7855</v>
+        <v>6857.7675</v>
       </c>
       <c r="D24" t="n">
         <v>33754.2325</v>
@@ -761,7 +734,7 @@
         <v>24</v>
       </c>
       <c r="C25" t="n">
-        <v>5494.996500000001</v>
+        <v>6096.6435</v>
       </c>
       <c r="D25" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Added DAP for today
</commit_message>
<xml_diff>
--- a/actual_energy.xlsx
+++ b/actual_energy.xlsx
@@ -448,13 +448,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>79488</v>
+        <v>36728</v>
       </c>
       <c r="C2" t="n">
-        <v>5597.0385765805</v>
+        <v>5799.800999999999</v>
       </c>
       <c r="D2" t="n">
-        <v>73890.9614234195</v>
+        <v>30928.199</v>
       </c>
     </row>
     <row r="3">
@@ -462,13 +462,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>75184</v>
+        <v>35269</v>
       </c>
       <c r="C3" t="n">
-        <v>5427.810091879</v>
+        <v>5649.136500000001</v>
       </c>
       <c r="D3" t="n">
-        <v>69756.189908121</v>
+        <v>29619.8635</v>
       </c>
     </row>
     <row r="4">
@@ -476,13 +476,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>71544</v>
+        <v>33348</v>
       </c>
       <c r="C4" t="n">
-        <v>5378.673491737501</v>
+        <v>5554.8325</v>
       </c>
       <c r="D4" t="n">
-        <v>66165.3265082625</v>
+        <v>27793.1675</v>
       </c>
     </row>
     <row r="5">
@@ -490,13 +490,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>69610</v>
+        <v>31700</v>
       </c>
       <c r="C5" t="n">
-        <v>5348.731399226001</v>
+        <v>5481.98</v>
       </c>
       <c r="D5" t="n">
-        <v>64261.268600774</v>
+        <v>26218.02</v>
       </c>
     </row>
     <row r="6">
@@ -504,13 +504,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>70806</v>
+        <v>30762</v>
       </c>
       <c r="C6" t="n">
-        <v>5372.321170922</v>
+        <v>5456.8815</v>
       </c>
       <c r="D6" t="n">
-        <v>65433.678829078</v>
+        <v>25305.1185</v>
       </c>
     </row>
     <row r="7">
@@ -518,13 +518,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>73348</v>
+        <v>30953</v>
       </c>
       <c r="C7" t="n">
-        <v>5496.759895401</v>
+        <v>5512.395</v>
       </c>
       <c r="D7" t="n">
-        <v>67851.240104599</v>
+        <v>25440.605</v>
       </c>
     </row>
     <row r="8">
@@ -532,13 +532,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>78137</v>
+        <v>31330</v>
       </c>
       <c r="C8" t="n">
-        <v>6441.069913339</v>
+        <v>5765.477227722772</v>
       </c>
       <c r="D8" t="n">
-        <v>71695.930086661</v>
+        <v>25564.52277227723</v>
       </c>
     </row>
     <row r="9">
@@ -546,13 +546,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>80939</v>
+        <v>32595</v>
       </c>
       <c r="C9" t="n">
-        <v>7184.668538918501</v>
+        <v>6519.4465</v>
       </c>
       <c r="D9" t="n">
-        <v>73754.3314610815</v>
+        <v>26075.5535</v>
       </c>
     </row>
     <row r="10">
@@ -560,13 +560,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>103039</v>
+        <v>36208</v>
       </c>
       <c r="C10" t="n">
-        <v>8465.353500000001</v>
+        <v>7901.5895</v>
       </c>
       <c r="D10" t="n">
-        <v>94573.6465</v>
+        <v>28306.4105</v>
       </c>
     </row>
     <row r="11">
@@ -574,13 +574,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>114408</v>
+        <v>39069</v>
       </c>
       <c r="C11" t="n">
-        <v>14333.5385</v>
+        <v>13052.0005</v>
       </c>
       <c r="D11" t="n">
-        <v>100074.4615</v>
+        <v>26016.9995</v>
       </c>
     </row>
     <row r="12">
@@ -588,145 +588,181 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>96449.10000000001</v>
+        <v>39884</v>
       </c>
       <c r="C12" t="n">
-        <v>15915.495</v>
+        <v>14886.7985</v>
       </c>
       <c r="D12" t="n">
-        <v>80533.60500000001</v>
+        <v>24997.2015</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
         <v>12</v>
       </c>
+      <c r="B13" t="n">
+        <v>39218</v>
+      </c>
       <c r="C13" t="n">
-        <v>15771.6165</v>
+        <v>14810.005</v>
       </c>
       <c r="D13" t="n">
-        <v>103987.3835</v>
+        <v>24407.995</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
         <v>13</v>
       </c>
+      <c r="B14" t="n">
+        <v>38683</v>
+      </c>
       <c r="C14" t="n">
-        <v>15824.06</v>
+        <v>14699.3385</v>
       </c>
       <c r="D14" t="n">
-        <v>76684.94</v>
+        <v>23983.6615</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
         <v>14</v>
       </c>
+      <c r="B15" t="n">
+        <v>40878</v>
+      </c>
       <c r="C15" t="n">
-        <v>15963.6205</v>
+        <v>15357.636</v>
       </c>
       <c r="D15" t="n">
-        <v>103417.3795</v>
+        <v>25520.364</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
         <v>15</v>
       </c>
+      <c r="B16" t="n">
+        <v>41508</v>
+      </c>
       <c r="C16" t="n">
-        <v>16132.936</v>
+        <v>15432.207</v>
       </c>
       <c r="D16" t="n">
-        <v>110937.064</v>
+        <v>26075.793</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
         <v>16</v>
       </c>
+      <c r="B17" t="n">
+        <v>40766</v>
+      </c>
       <c r="C17" t="n">
-        <v>16102.835</v>
+        <v>15338.9075</v>
       </c>
       <c r="D17" t="n">
-        <v>87260.16500000001</v>
+        <v>25427.0925</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
         <v>17</v>
       </c>
+      <c r="B18" t="n">
+        <v>38994</v>
+      </c>
       <c r="C18" t="n">
-        <v>16787.6375</v>
+        <v>15792.80217625723</v>
       </c>
       <c r="D18" t="n">
-        <v>81550.3625</v>
+        <v>23201.19782374277</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
         <v>18</v>
       </c>
+      <c r="B19" t="n">
+        <v>39323</v>
+      </c>
       <c r="C19" t="n">
-        <v>16403.816</v>
+        <v>15557.50171551809</v>
       </c>
       <c r="D19" t="n">
-        <v>75216.18400000001</v>
+        <v>23765.49828448191</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
         <v>19</v>
       </c>
+      <c r="B20" t="n">
+        <v>41039</v>
+      </c>
       <c r="C20" t="n">
-        <v>16006.496</v>
+        <v>15152.49877462994</v>
       </c>
       <c r="D20" t="n">
-        <v>71081.504</v>
+        <v>25886.50122537006</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
         <v>20</v>
       </c>
+      <c r="B21" t="n">
+        <v>38646</v>
+      </c>
       <c r="C21" t="n">
-        <v>14046.071</v>
+        <v>13812.90902852661</v>
       </c>
       <c r="D21" t="n">
-        <v>69127.929</v>
+        <v>24833.09097147339</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
         <v>21</v>
       </c>
+      <c r="B22" t="n">
+        <v>38253</v>
+      </c>
       <c r="C22" t="n">
-        <v>11183.005</v>
+        <v>12007.84432898735</v>
       </c>
       <c r="D22" t="n">
-        <v>68523.995</v>
+        <v>26245.15567101265</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
         <v>22</v>
       </c>
+      <c r="B23" t="n">
+        <v>38679</v>
+      </c>
       <c r="C23" t="n">
-        <v>9240.505000000001</v>
+        <v>9523.143</v>
       </c>
       <c r="D23" t="n">
-        <v>66852.495</v>
+        <v>29155.857</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
         <v>23</v>
       </c>
+      <c r="B24" t="n">
+        <v>38098</v>
+      </c>
       <c r="C24" t="n">
-        <v>6857.7675</v>
+        <v>6375.7855</v>
       </c>
       <c r="D24" t="n">
-        <v>33754.2325</v>
+        <v>31722.2145</v>
       </c>
     </row>
     <row r="25">
@@ -734,7 +770,7 @@
         <v>24</v>
       </c>
       <c r="C25" t="n">
-        <v>6096.6435</v>
+        <v>5494.996500000001</v>
       </c>
       <c r="D25" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Added DAP file for today
</commit_message>
<xml_diff>
--- a/actual_energy.xlsx
+++ b/actual_energy.xlsx
@@ -574,13 +574,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>12258</v>
+        <v>32621</v>
       </c>
       <c r="C11" t="n">
         <v>13169.898</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>19451.102</v>
       </c>
     </row>
     <row r="12">
@@ -588,134 +588,167 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>6128</v>
+        <v>33187</v>
       </c>
       <c r="C12" t="n">
         <v>15125.579</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>18061.421</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
         <v>12</v>
       </c>
+      <c r="B13" t="n">
+        <v>32997</v>
+      </c>
       <c r="C13" t="n">
         <v>14795.5535</v>
       </c>
       <c r="D13" t="n">
-        <v>24422.4465</v>
+        <v>18201.4465</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
         <v>13</v>
       </c>
+      <c r="B14" t="n">
+        <v>34647</v>
+      </c>
       <c r="C14" t="n">
         <v>15027.4215</v>
       </c>
       <c r="D14" t="n">
-        <v>23655.5785</v>
+        <v>19619.5785</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
         <v>14</v>
       </c>
+      <c r="B15" t="n">
+        <v>35793</v>
+      </c>
       <c r="C15" t="n">
         <v>15238.5275</v>
       </c>
       <c r="D15" t="n">
-        <v>25639.4725</v>
+        <v>20554.4725</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
         <v>15</v>
       </c>
+      <c r="B16" t="n">
+        <v>37060</v>
+      </c>
       <c r="C16" t="n">
         <v>15218.588</v>
       </c>
       <c r="D16" t="n">
-        <v>26289.412</v>
+        <v>21841.412</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
         <v>16</v>
       </c>
+      <c r="B17" t="n">
+        <v>37376</v>
+      </c>
       <c r="C17" t="n">
         <v>15079.778</v>
       </c>
       <c r="D17" t="n">
-        <v>25686.222</v>
+        <v>22296.222</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
         <v>17</v>
       </c>
+      <c r="B18" t="n">
+        <v>37480</v>
+      </c>
       <c r="C18" t="n">
         <v>15600.9735</v>
       </c>
       <c r="D18" t="n">
-        <v>23393.0265</v>
+        <v>21879.0265</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
         <v>18</v>
       </c>
+      <c r="B19" t="n">
+        <v>40256</v>
+      </c>
       <c r="C19" t="n">
         <v>15471.0605</v>
       </c>
       <c r="D19" t="n">
-        <v>23851.9395</v>
+        <v>24784.9395</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
         <v>19</v>
       </c>
+      <c r="B20" t="n">
+        <v>42234</v>
+      </c>
       <c r="C20" t="n">
         <v>15033.3155</v>
       </c>
       <c r="D20" t="n">
-        <v>26005.6845</v>
+        <v>27200.6845</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
         <v>20</v>
       </c>
+      <c r="B21" t="n">
+        <v>40306</v>
+      </c>
       <c r="C21" t="n">
         <v>13476.9705</v>
       </c>
       <c r="D21" t="n">
-        <v>25169.0295</v>
+        <v>26829.0295</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
         <v>21</v>
       </c>
+      <c r="B22" t="n">
+        <v>40825</v>
+      </c>
       <c r="C22" t="n">
         <v>11646.733</v>
       </c>
       <c r="D22" t="n">
-        <v>26606.267</v>
+        <v>29178.267</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
         <v>22</v>
       </c>
+      <c r="B23" t="n">
+        <v>41147</v>
+      </c>
       <c r="C23" t="n">
         <v>9235.5095</v>
       </c>
       <c r="D23" t="n">
-        <v>29443.4905</v>
+        <v>31911.4905</v>
       </c>
     </row>
     <row r="24">

</xml_diff>